<commit_message>
Fix DB bug - Exam Admin
</commit_message>
<xml_diff>
--- a/OAES Database Design.xlsx
+++ b/OAES Database Design.xlsx
@@ -10,8 +10,8 @@
   <sheets>
     <sheet name="OAES_USER_MGMT" sheetId="1" state="visible" r:id="rId2"/>
     <sheet name="OAES_AUTHORING" sheetId="2" state="visible" r:id="rId3"/>
-    <sheet name="OAES_ASSESSMENT" sheetId="3" state="visible" r:id="rId4"/>
-    <sheet name="OEAS_EXAM_ADMIN" sheetId="4" state="visible" r:id="rId5"/>
+    <sheet name="OEAS_EXAM_ADMIN" sheetId="3" state="visible" r:id="rId4"/>
+    <sheet name="OAES_ASSESSMENT" sheetId="4" state="visible" r:id="rId5"/>
     <sheet name="OAES_EVAL" sheetId="5" state="visible" r:id="rId6"/>
   </sheets>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.0001"/>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="298" uniqueCount="155">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="299" uniqueCount="156">
   <si>
     <t xml:space="preserve">oaes_user</t>
   </si>
@@ -242,12 +242,159 @@
     <t xml:space="preserve">examinee_batch</t>
   </si>
   <si>
+    <t xml:space="preserve">instruction</t>
+  </si>
+  <si>
+    <t xml:space="preserve">examinee_item_marks</t>
+  </si>
+  <si>
+    <t xml:space="preserve">course_master_id PK</t>
+  </si>
+  <si>
+    <t xml:space="preserve">examdrive_id PK</t>
+  </si>
+  <si>
+    <t xml:space="preserve">examinee_id PK</t>
+  </si>
+  <si>
+    <t xml:space="preserve">center_id PK</t>
+  </si>
+  <si>
+    <t xml:space="preserve">batch_id PK</t>
+  </si>
+  <si>
+    <t xml:space="preserve">examinee_batch_id PK</t>
+  </si>
+  <si>
+    <t xml:space="preserve">instruction_id PK</t>
+  </si>
+  <si>
+    <t xml:space="preserve">examinee_item_marks_id PK</t>
+  </si>
+  <si>
+    <t xml:space="preserve">examdrive_name</t>
+  </si>
+  <si>
+    <t xml:space="preserve">examinee_name</t>
+  </si>
+  <si>
+    <t xml:space="preserve">center_name</t>
+  </si>
+  <si>
+    <t xml:space="preserve">center_id refers CENTER</t>
+  </si>
+  <si>
+    <t xml:space="preserve">marks_obtained</t>
+  </si>
+  <si>
+    <t xml:space="preserve">batch_id FK refers BATCH</t>
+  </si>
+  <si>
+    <t xml:space="preserve">qp_id FK refers QUESTION_PAPER</t>
+  </si>
+  <si>
+    <t xml:space="preserve">itemtype_name</t>
+  </si>
+  <si>
+    <t xml:space="preserve">qp_item_id FK refers QP_ITEM</t>
+  </si>
+  <si>
+    <t xml:space="preserve">course_code UNIQUE NOTNULL</t>
+  </si>
+  <si>
+    <t xml:space="preserve">status ( NOT STARTED, IN_PROGRESS, COMPLETED)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">examinee_password</t>
+  </si>
+  <si>
+    <t xml:space="preserve">center_code UNIQUE NOTNULL</t>
+  </si>
+  <si>
+    <t xml:space="preserve">batch_start_time</t>
+  </si>
+  <si>
+    <t xml:space="preserve">examinee_id FK refers EXAMINEE</t>
+  </si>
+  <si>
+    <t xml:space="preserve">maximum_marks</t>
+  </si>
+  <si>
+    <t xml:space="preserve">instruction_code UNIQUE NOTNULL</t>
+  </si>
+  <si>
+    <t xml:space="preserve">itemtype_category (AUTO, MANUAL)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">examinee_batch_id FK refers EXAMINEE_BATCH</t>
+  </si>
+  <si>
+    <t xml:space="preserve">true_percentage</t>
+  </si>
+  <si>
+    <t xml:space="preserve">exam_drive_code UNIQUE NOTNULL</t>
+  </si>
+  <si>
+    <t xml:space="preserve">examinee_code UNIQUE NOTNULL</t>
+  </si>
+  <si>
+    <t xml:space="preserve">center_capacity</t>
+  </si>
+  <si>
+    <t xml:space="preserve">batch_end_time</t>
+  </si>
+  <si>
+    <t xml:space="preserve">duration</t>
+  </si>
+  <si>
+    <t xml:space="preserve">instruction_text</t>
+  </si>
+  <si>
+    <t xml:space="preserve">itemtype_code UNIQUE NOTNULL</t>
+  </si>
+  <si>
+    <t xml:space="preserve">mcq_option_percentage</t>
+  </si>
+  <si>
+    <t xml:space="preserve">false_percentage</t>
+  </si>
+  <si>
+    <t xml:space="preserve">course_master_id FK refers COURSE_MASTER</t>
+  </si>
+  <si>
+    <t xml:space="preserve">examinee_branch</t>
+  </si>
+  <si>
+    <t xml:space="preserve">batch_code UNIQUE NOTNULL</t>
+  </si>
+  <si>
+    <t xml:space="preserve">qp_code UNIQUE NOTNULL</t>
+  </si>
+  <si>
+    <t xml:space="preserve">item_mcq_options_code UNIQUE NOTNULL</t>
+  </si>
+  <si>
+    <t xml:space="preserve">item_true_false_code UNIQUE NOTNULL</t>
+  </si>
+  <si>
+    <t xml:space="preserve">examinee_email</t>
+  </si>
+  <si>
+    <t xml:space="preserve">qp_status(PENDING,RECEIVED,ERROR_SENDING)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">examinee_college</t>
+  </si>
+  <si>
+    <t xml:space="preserve">course_master_id refers COURSE_MASTER</t>
+  </si>
+  <si>
+    <t xml:space="preserve">item_code UNIQUE NOTNULL</t>
+  </si>
+  <si>
     <t xml:space="preserve">invigilator</t>
   </si>
   <si>
-    <t xml:space="preserve">instruction</t>
-  </si>
-  <si>
     <t xml:space="preserve">attempt</t>
   </si>
   <si>
@@ -260,30 +407,9 @@
     <t xml:space="preserve">response_true_false</t>
   </si>
   <si>
-    <t xml:space="preserve">course_master_id PK</t>
-  </si>
-  <si>
-    <t xml:space="preserve">examdrive_id PK</t>
-  </si>
-  <si>
-    <t xml:space="preserve">examinee_id PK</t>
-  </si>
-  <si>
-    <t xml:space="preserve">center_id PK</t>
-  </si>
-  <si>
-    <t xml:space="preserve">batch_id PK</t>
-  </si>
-  <si>
-    <t xml:space="preserve">examinee_batch_id PK</t>
-  </si>
-  <si>
     <t xml:space="preserve">invigilator_id PK</t>
   </si>
   <si>
-    <t xml:space="preserve">instruction_id PK</t>
-  </si>
-  <si>
     <t xml:space="preserve">attempt_id PK</t>
   </si>
   <si>
@@ -296,75 +422,18 @@
     <t xml:space="preserve">response_true_false_id PK</t>
   </si>
   <si>
-    <t xml:space="preserve">examdrive_name</t>
-  </si>
-  <si>
-    <t xml:space="preserve">examinee_name</t>
-  </si>
-  <si>
-    <t xml:space="preserve">center_name</t>
-  </si>
-  <si>
-    <t xml:space="preserve">center_id refers CENTER</t>
-  </si>
-  <si>
-    <t xml:space="preserve">batch_id FK refers BATCH</t>
-  </si>
-  <si>
     <t xml:space="preserve">invigilator_name</t>
   </si>
   <si>
-    <t xml:space="preserve">qp_id FK refers QUESTION_PAPER</t>
-  </si>
-  <si>
-    <t xml:space="preserve">itemtype_name</t>
-  </si>
-  <si>
-    <t xml:space="preserve">item_code UNIQUE NOTNULL</t>
-  </si>
-  <si>
-    <t xml:space="preserve">qp_item_id FK refers QP_ITEM</t>
-  </si>
-  <si>
     <t xml:space="preserve">attempt_number</t>
   </si>
   <si>
     <t xml:space="preserve">response_id FK referes RESPONSE</t>
   </si>
   <si>
-    <t xml:space="preserve">course_code UNIQUE NOTNULL</t>
-  </si>
-  <si>
-    <t xml:space="preserve">status ( NOT STARTED, IN_PROGRESS, COMPLETED)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">examinee_password</t>
-  </si>
-  <si>
-    <t xml:space="preserve">center_code UNIQUE NOTNULL</t>
-  </si>
-  <si>
-    <t xml:space="preserve">batch_start_time</t>
-  </si>
-  <si>
-    <t xml:space="preserve">examinee_id FK refers EXAMINEE</t>
-  </si>
-  <si>
     <t xml:space="preserve">invigilator_email</t>
   </si>
   <si>
-    <t xml:space="preserve">maximum_marks</t>
-  </si>
-  <si>
-    <t xml:space="preserve">instruction_code UNIQUE NOTNULL</t>
-  </si>
-  <si>
-    <t xml:space="preserve">itemtype_category (AUTO, MANUAL)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">item_true_false_code UNIQUE NOTNULL</t>
-  </si>
-  <si>
     <t xml:space="preserve">status (NOT_Started, IN_Progress,Completed,Abandoned )</t>
   </si>
   <si>
@@ -377,33 +446,9 @@
     <t xml:space="preserve">response_true_false_code UNIQUE NOTNULL</t>
   </si>
   <si>
-    <t xml:space="preserve">exam_drive_code UNIQUE NOTNULL</t>
-  </si>
-  <si>
-    <t xml:space="preserve">examinee_code UNIQUE NOTNULL</t>
-  </si>
-  <si>
-    <t xml:space="preserve">center_capacity</t>
-  </si>
-  <si>
-    <t xml:space="preserve">batch_end_time</t>
-  </si>
-  <si>
     <t xml:space="preserve">invigilator_password</t>
   </si>
   <si>
-    <t xml:space="preserve">duration</t>
-  </si>
-  <si>
-    <t xml:space="preserve">instruction_text</t>
-  </si>
-  <si>
-    <t xml:space="preserve">itemtype_code UNIQUE NOTNULL</t>
-  </si>
-  <si>
-    <t xml:space="preserve">item_mcq_options_code UNIQUE NOTNULL</t>
-  </si>
-  <si>
     <t xml:space="preserve">attempt_start_time</t>
   </si>
   <si>
@@ -413,61 +458,19 @@
     <t xml:space="preserve">response_mcq_code UNIQUE NOTNULL</t>
   </si>
   <si>
-    <t xml:space="preserve">course_master_id FK refers COURSE_MASTER</t>
-  </si>
-  <si>
-    <t xml:space="preserve">examinee_branch</t>
-  </si>
-  <si>
-    <t xml:space="preserve">batch_code UNIQUE NOTNULL</t>
-  </si>
-  <si>
     <t xml:space="preserve">batch_id FK refers BATCH_COURSE</t>
   </si>
   <si>
-    <t xml:space="preserve">qp_code UNIQUE NOTNULL</t>
-  </si>
-  <si>
     <t xml:space="preserve">attempt_end_time</t>
   </si>
   <si>
-    <t xml:space="preserve">examinee_college</t>
-  </si>
-  <si>
     <t xml:space="preserve">user_status(Active, NOT_Active)</t>
   </si>
   <si>
-    <t xml:space="preserve">examinee_batch_id FK refers EXAMINEE_BATCH</t>
-  </si>
-  <si>
     <t xml:space="preserve">invigilator_code UNIQUE NOTNULL</t>
   </si>
   <si>
     <t xml:space="preserve">attempt_code UNIQUE NOTNULL</t>
-  </si>
-  <si>
-    <t xml:space="preserve">examinee_item_marks</t>
-  </si>
-  <si>
-    <t xml:space="preserve">examinee_item_marks_id PK</t>
-  </si>
-  <si>
-    <t xml:space="preserve">marks_obtained</t>
-  </si>
-  <si>
-    <t xml:space="preserve">true_percentage</t>
-  </si>
-  <si>
-    <t xml:space="preserve">mcq_option_percentage</t>
-  </si>
-  <si>
-    <t xml:space="preserve">false_percentage</t>
-  </si>
-  <si>
-    <t xml:space="preserve">examinee_email</t>
-  </si>
-  <si>
-    <t xml:space="preserve">qp_status(PENDING,RECEIVED,ERROR_SENDING)</t>
   </si>
   <si>
     <t xml:space="preserve">drive_center_examinee</t>
@@ -498,7 +501,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="General"/>
   </numFmts>
-  <fonts count="12">
+  <fonts count="11">
     <font>
       <sz val="10"/>
       <color rgb="FF000000"/>
@@ -537,6 +540,13 @@
       <charset val="1"/>
     </font>
     <font>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Arial"/>
+      <family val="0"/>
+      <charset val="1"/>
+    </font>
+    <font>
       <b val="true"/>
       <sz val="11"/>
       <color rgb="FF000000"/>
@@ -547,22 +557,9 @@
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
-      <name val="Arial"/>
-      <family val="0"/>
-      <charset val="1"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF000000"/>
       <name val="Calibri"/>
       <family val="0"/>
       <charset val="1"/>
-    </font>
-    <font>
-      <sz val="10"/>
-      <color rgb="FF000000"/>
-      <name val="Calibri"/>
-      <family val="0"/>
     </font>
     <font>
       <sz val="11"/>
@@ -633,6 +630,13 @@
       <diagonal/>
     </border>
     <border diagonalUp="false" diagonalDown="false">
+      <left style="hair"/>
+      <right style="hair"/>
+      <top style="hair"/>
+      <bottom style="hair"/>
+      <diagonal/>
+    </border>
+    <border diagonalUp="false" diagonalDown="false">
       <left style="thin"/>
       <right style="thin"/>
       <top/>
@@ -644,13 +648,6 @@
       <right style="thin"/>
       <top/>
       <bottom style="thin"/>
-      <diagonal/>
-    </border>
-    <border diagonalUp="false" diagonalDown="false">
-      <left style="hair"/>
-      <right style="hair"/>
-      <top style="hair"/>
-      <bottom style="hair"/>
       <diagonal/>
     </border>
   </borders>
@@ -679,7 +676,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="30">
+  <cellXfs count="28">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -712,23 +709,35 @@
       <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="6" fillId="2" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="6" fillId="2" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="6" fillId="2" borderId="3" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="6" fillId="4" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="5" fillId="4" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="7" fillId="2" borderId="3" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="8" fillId="3" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="7" fillId="2" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="7" fillId="2" borderId="4" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -736,47 +745,27 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="9" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="10" fillId="0" borderId="3" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="8" fillId="3" borderId="4" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="7" fillId="0" borderId="3" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="9" fillId="0" borderId="4" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="6" fillId="0" borderId="4" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="7" fillId="4" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="7" fillId="5" borderId="3" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="7" fillId="5" borderId="4" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="5" fillId="4" borderId="4" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="6" fillId="5" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="6" fillId="5" borderId="3" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="11" fillId="4" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="10" fillId="4" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -784,30 +773,30 @@
       <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="7" fillId="4" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="6" fillId="4" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="7" fillId="4" borderId="3" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="6" fillId="4" borderId="4" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="8" fillId="4" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="8" fillId="4" borderId="3" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="7" fillId="4" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="6" fillId="4" borderId="3" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
   </cellXfs>
   <cellStyles count="6">
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
-    <cellStyle name="Comma" xfId="15" builtinId="3"/>
-    <cellStyle name="Comma [0]" xfId="16" builtinId="6"/>
-    <cellStyle name="Currency" xfId="17" builtinId="4"/>
-    <cellStyle name="Currency [0]" xfId="18" builtinId="7"/>
-    <cellStyle name="Percent" xfId="19" builtinId="5"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0" customBuiltin="false"/>
+    <cellStyle name="Comma" xfId="15" builtinId="3" customBuiltin="false"/>
+    <cellStyle name="Comma [0]" xfId="16" builtinId="6" customBuiltin="false"/>
+    <cellStyle name="Currency" xfId="17" builtinId="4" customBuiltin="false"/>
+    <cellStyle name="Currency [0]" xfId="18" builtinId="7" customBuiltin="false"/>
+    <cellStyle name="Percent" xfId="19" builtinId="5" customBuiltin="false"/>
   </cellStyles>
   <dxfs count="1">
     <dxf>
@@ -1510,387 +1499,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:Q8"/>
+  <dimension ref="A1:AC14"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="K13" activeCellId="0" sqref="K13"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
-  <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="24.64"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="39.09"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="26.82"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="24.45"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="23.91"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="26.18"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="0" width="27.64"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="0" width="21.82"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="0" width="27.55"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="0" width="29.1"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="11" min="11" style="0" width="61.92"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="12" min="12" style="0" width="33.37"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="13" min="13" style="0" width="31.82"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="14" min="14" style="0" width="45.01"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="15" min="15" style="0" width="26.55"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="16" min="16" style="0" width="30.36"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="17" min="17" style="0" width="38.1"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="18" min="18" style="0" width="31.69"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="19" min="19" style="0" width="36.31"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="21" min="20" style="0" width="27.12"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="22" min="22" style="0" width="20.14"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="23" min="23" style="0" width="36.57"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="24" min="24" style="0" width="19.71"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="25" min="25" style="0" width="36.71"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="26" style="0" width="14.43"/>
-  </cols>
-  <sheetData>
-    <row r="1" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="7" t="s">
-        <v>66</v>
-      </c>
-      <c r="B1" s="7" t="s">
-        <v>67</v>
-      </c>
-      <c r="C1" s="7" t="s">
-        <v>68</v>
-      </c>
-      <c r="D1" s="7" t="s">
-        <v>69</v>
-      </c>
-      <c r="E1" s="7" t="s">
-        <v>70</v>
-      </c>
-      <c r="F1" s="7" t="s">
-        <v>71</v>
-      </c>
-      <c r="G1" s="7" t="s">
-        <v>72</v>
-      </c>
-      <c r="H1" s="7" t="s">
-        <v>28</v>
-      </c>
-      <c r="I1" s="7" t="s">
-        <v>73</v>
-      </c>
-      <c r="J1" s="7" t="s">
-        <v>23</v>
-      </c>
-      <c r="K1" s="8" t="s">
-        <v>29</v>
-      </c>
-      <c r="L1" s="7" t="s">
-        <v>26</v>
-      </c>
-      <c r="M1" s="7" t="s">
-        <v>27</v>
-      </c>
-      <c r="N1" s="9" t="s">
-        <v>74</v>
-      </c>
-      <c r="O1" s="1" t="s">
-        <v>75</v>
-      </c>
-      <c r="P1" s="10" t="s">
-        <v>76</v>
-      </c>
-      <c r="Q1" s="10" t="s">
-        <v>77</v>
-      </c>
-    </row>
-    <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="2" t="s">
-        <v>78</v>
-      </c>
-      <c r="B2" s="2" t="s">
-        <v>79</v>
-      </c>
-      <c r="C2" s="2" t="s">
-        <v>80</v>
-      </c>
-      <c r="D2" s="2" t="s">
-        <v>81</v>
-      </c>
-      <c r="E2" s="2" t="s">
-        <v>82</v>
-      </c>
-      <c r="F2" s="11" t="s">
-        <v>83</v>
-      </c>
-      <c r="G2" s="2" t="s">
-        <v>84</v>
-      </c>
-      <c r="H2" s="2" t="s">
-        <v>38</v>
-      </c>
-      <c r="I2" s="2" t="s">
-        <v>85</v>
-      </c>
-      <c r="J2" s="2" t="s">
-        <v>33</v>
-      </c>
-      <c r="K2" s="12" t="s">
-        <v>39</v>
-      </c>
-      <c r="L2" s="2" t="s">
-        <v>36</v>
-      </c>
-      <c r="M2" s="2" t="s">
-        <v>37</v>
-      </c>
-      <c r="N2" s="12" t="s">
-        <v>86</v>
-      </c>
-      <c r="O2" s="2" t="s">
-        <v>87</v>
-      </c>
-      <c r="P2" s="13" t="s">
-        <v>88</v>
-      </c>
-      <c r="Q2" s="13" t="s">
-        <v>89</v>
-      </c>
-    </row>
-    <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="2" t="s">
-        <v>40</v>
-      </c>
-      <c r="B3" s="2" t="s">
-        <v>90</v>
-      </c>
-      <c r="C3" s="2" t="s">
-        <v>91</v>
-      </c>
-      <c r="D3" s="2" t="s">
-        <v>92</v>
-      </c>
-      <c r="E3" s="2" t="s">
-        <v>93</v>
-      </c>
-      <c r="F3" s="14" t="s">
-        <v>94</v>
-      </c>
-      <c r="G3" s="2" t="s">
-        <v>95</v>
-      </c>
-      <c r="H3" s="2" t="s">
-        <v>94</v>
-      </c>
-      <c r="I3" s="2" t="s">
-        <v>96</v>
-      </c>
-      <c r="J3" s="2" t="s">
-        <v>97</v>
-      </c>
-      <c r="K3" s="12" t="s">
-        <v>98</v>
-      </c>
-      <c r="L3" s="2" t="s">
-        <v>99</v>
-      </c>
-      <c r="M3" s="2" t="s">
-        <v>99</v>
-      </c>
-      <c r="N3" s="12" t="s">
-        <v>100</v>
-      </c>
-      <c r="O3" s="2" t="s">
-        <v>99</v>
-      </c>
-      <c r="P3" s="13" t="s">
-        <v>101</v>
-      </c>
-      <c r="Q3" s="13" t="s">
-        <v>101</v>
-      </c>
-    </row>
-    <row r="4" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="2" t="s">
-        <v>102</v>
-      </c>
-      <c r="B4" s="2" t="s">
-        <v>103</v>
-      </c>
-      <c r="C4" s="2" t="s">
-        <v>104</v>
-      </c>
-      <c r="D4" s="2" t="s">
-        <v>105</v>
-      </c>
-      <c r="E4" s="2" t="s">
-        <v>106</v>
-      </c>
-      <c r="F4" s="2" t="s">
-        <v>107</v>
-      </c>
-      <c r="G4" s="2" t="s">
-        <v>108</v>
-      </c>
-      <c r="H4" s="2" t="s">
-        <v>109</v>
-      </c>
-      <c r="I4" s="2" t="s">
-        <v>110</v>
-      </c>
-      <c r="J4" s="2" t="s">
-        <v>111</v>
-      </c>
-      <c r="K4" s="2" t="s">
-        <v>96</v>
-      </c>
-      <c r="L4" s="2" t="s">
-        <v>51</v>
-      </c>
-      <c r="M4" s="14" t="s">
-        <v>112</v>
-      </c>
-      <c r="N4" s="2" t="s">
-        <v>113</v>
-      </c>
-      <c r="O4" s="2" t="s">
-        <v>114</v>
-      </c>
-      <c r="P4" s="13" t="s">
-        <v>115</v>
-      </c>
-      <c r="Q4" s="13" t="s">
-        <v>116</v>
-      </c>
-    </row>
-    <row r="5" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="2"/>
-      <c r="B5" s="2" t="s">
-        <v>117</v>
-      </c>
-      <c r="C5" s="2" t="s">
-        <v>118</v>
-      </c>
-      <c r="D5" s="2" t="s">
-        <v>119</v>
-      </c>
-      <c r="E5" s="2" t="s">
-        <v>120</v>
-      </c>
-      <c r="F5" s="2"/>
-      <c r="G5" s="3" t="s">
-        <v>121</v>
-      </c>
-      <c r="H5" s="2" t="s">
-        <v>122</v>
-      </c>
-      <c r="I5" s="2" t="s">
-        <v>123</v>
-      </c>
-      <c r="J5" s="2" t="s">
-        <v>124</v>
-      </c>
-      <c r="K5" s="2" t="s">
-        <v>49</v>
-      </c>
-      <c r="L5" s="14" t="s">
-        <v>125</v>
-      </c>
-      <c r="M5" s="2"/>
-      <c r="N5" s="2" t="s">
-        <v>126</v>
-      </c>
-      <c r="O5" s="2" t="s">
-        <v>127</v>
-      </c>
-      <c r="P5" s="2" t="s">
-        <v>128</v>
-      </c>
-      <c r="Q5" s="15"/>
-    </row>
-    <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A6" s="2"/>
-      <c r="B6" s="2" t="s">
-        <v>129</v>
-      </c>
-      <c r="C6" s="2" t="s">
-        <v>130</v>
-      </c>
-      <c r="D6" s="2"/>
-      <c r="E6" s="2" t="s">
-        <v>131</v>
-      </c>
-      <c r="F6" s="2"/>
-      <c r="G6" s="2" t="s">
-        <v>132</v>
-      </c>
-      <c r="H6" s="2" t="s">
-        <v>133</v>
-      </c>
-      <c r="I6" s="2"/>
-      <c r="J6" s="2"/>
-      <c r="K6" s="2" t="s">
-        <v>59</v>
-      </c>
-      <c r="L6" s="2"/>
-      <c r="M6" s="2"/>
-      <c r="N6" s="2" t="s">
-        <v>134</v>
-      </c>
-      <c r="O6" s="16"/>
-      <c r="P6" s="16"/>
-      <c r="Q6" s="16"/>
-    </row>
-    <row r="7" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C7" s="2" t="s">
-        <v>135</v>
-      </c>
-      <c r="G7" s="2" t="s">
-        <v>136</v>
-      </c>
-      <c r="K7" s="2" t="s">
-        <v>55</v>
-      </c>
-      <c r="N7" s="2" t="s">
-        <v>137</v>
-      </c>
-      <c r="O7" s="16"/>
-      <c r="P7" s="17"/>
-      <c r="Q7" s="17"/>
-    </row>
-    <row r="8" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="G8" s="2" t="s">
-        <v>138</v>
-      </c>
-      <c r="K8" s="2" t="s">
-        <v>61</v>
-      </c>
-      <c r="N8" s="2" t="s">
-        <v>139</v>
-      </c>
-      <c r="O8" s="16"/>
-      <c r="P8" s="17"/>
-      <c r="Q8" s="17"/>
-    </row>
-  </sheetData>
-  <conditionalFormatting sqref="G2:G7 K8 N8">
-    <cfRule type="expression" priority="2" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="0">
-      <formula>LEN(TRIM(#REF!))&gt;0</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
-  <pageMargins left="0.747916666666667" right="0.747916666666667" top="0.984027777777778" bottom="0.984027777777778" header="0.511805555555555" footer="0.511805555555555"/>
-  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
-  <headerFooter differentFirst="false" differentOddEven="false">
-    <oddHeader/>
-    <oddFooter/>
-  </headerFooter>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <sheetPr filterMode="false">
-    <pageSetUpPr fitToPage="false"/>
-  </sheetPr>
-  <dimension ref="A1:AC998"/>
-  <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="J16" activeCellId="0" sqref="J16"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="D1" colorId="64" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="E17" activeCellId="0" sqref="E17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -1935,7 +1547,7 @@
         <v>28</v>
       </c>
       <c r="H1" s="7" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="I1" s="7" t="s">
         <v>23</v>
@@ -1944,7 +1556,7 @@
         <v>29</v>
       </c>
       <c r="K1" s="7" t="s">
-        <v>140</v>
+        <v>73</v>
       </c>
       <c r="L1" s="7" t="s">
         <v>26</v>
@@ -1952,47 +1564,47 @@
       <c r="M1" s="7" t="s">
         <v>27</v>
       </c>
-      <c r="N1" s="18"/>
-      <c r="O1" s="18"/>
-      <c r="P1" s="18"/>
-      <c r="Q1" s="18"/>
-      <c r="R1" s="18"/>
-      <c r="S1" s="18"/>
-      <c r="T1" s="18"/>
-      <c r="U1" s="18"/>
-      <c r="V1" s="18"/>
-      <c r="W1" s="18"/>
-      <c r="X1" s="18"/>
-      <c r="Y1" s="18"/>
-      <c r="Z1" s="18"/>
-      <c r="AA1" s="18"/>
-      <c r="AB1" s="18"/>
-      <c r="AC1" s="18"/>
+      <c r="N1" s="8"/>
+      <c r="O1" s="8"/>
+      <c r="P1" s="8"/>
+      <c r="Q1" s="8"/>
+      <c r="R1" s="8"/>
+      <c r="S1" s="8"/>
+      <c r="T1" s="8"/>
+      <c r="U1" s="8"/>
+      <c r="V1" s="8"/>
+      <c r="W1" s="8"/>
+      <c r="X1" s="8"/>
+      <c r="Y1" s="8"/>
+      <c r="Z1" s="8"/>
+      <c r="AA1" s="8"/>
+      <c r="AB1" s="8"/>
+      <c r="AC1" s="8"/>
     </row>
     <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="2" t="s">
+        <v>74</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>75</v>
+      </c>
+      <c r="C2" s="2" t="s">
+        <v>76</v>
+      </c>
+      <c r="D2" s="2" t="s">
+        <v>77</v>
+      </c>
+      <c r="E2" s="2" t="s">
         <v>78</v>
       </c>
-      <c r="B2" s="2" t="s">
+      <c r="F2" s="9" t="s">
         <v>79</v>
-      </c>
-      <c r="C2" s="2" t="s">
-        <v>80</v>
-      </c>
-      <c r="D2" s="2" t="s">
-        <v>81</v>
-      </c>
-      <c r="E2" s="2" t="s">
-        <v>82</v>
-      </c>
-      <c r="F2" s="11" t="s">
-        <v>83</v>
       </c>
       <c r="G2" s="2" t="s">
         <v>38</v>
       </c>
       <c r="H2" s="2" t="s">
-        <v>85</v>
+        <v>80</v>
       </c>
       <c r="I2" s="2" t="s">
         <v>33</v>
@@ -2001,7 +1613,7 @@
         <v>39</v>
       </c>
       <c r="K2" s="2" t="s">
-        <v>141</v>
+        <v>81</v>
       </c>
       <c r="L2" s="2" t="s">
         <v>36</v>
@@ -2009,246 +1621,246 @@
       <c r="M2" s="2" t="s">
         <v>37</v>
       </c>
-      <c r="N2" s="18"/>
-      <c r="O2" s="18"/>
-      <c r="P2" s="18"/>
-      <c r="Q2" s="18"/>
-      <c r="R2" s="18"/>
-      <c r="S2" s="18"/>
-      <c r="T2" s="18"/>
-      <c r="U2" s="18"/>
-      <c r="V2" s="18"/>
-      <c r="W2" s="18"/>
-      <c r="X2" s="18"/>
-      <c r="Y2" s="18"/>
-      <c r="Z2" s="18"/>
-      <c r="AA2" s="18"/>
-      <c r="AB2" s="18"/>
-      <c r="AC2" s="18"/>
+      <c r="N2" s="8"/>
+      <c r="O2" s="8"/>
+      <c r="P2" s="8"/>
+      <c r="Q2" s="8"/>
+      <c r="R2" s="8"/>
+      <c r="S2" s="8"/>
+      <c r="T2" s="8"/>
+      <c r="U2" s="8"/>
+      <c r="V2" s="8"/>
+      <c r="W2" s="8"/>
+      <c r="X2" s="8"/>
+      <c r="Y2" s="8"/>
+      <c r="Z2" s="8"/>
+      <c r="AA2" s="8"/>
+      <c r="AB2" s="8"/>
+      <c r="AC2" s="8"/>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="2" t="s">
         <v>40</v>
       </c>
       <c r="B3" s="2" t="s">
+        <v>82</v>
+      </c>
+      <c r="C3" s="2" t="s">
+        <v>83</v>
+      </c>
+      <c r="D3" s="2" t="s">
+        <v>84</v>
+      </c>
+      <c r="E3" s="2" t="s">
+        <v>85</v>
+      </c>
+      <c r="F3" s="2" t="s">
+        <v>86</v>
+      </c>
+      <c r="G3" s="2" t="s">
+        <v>87</v>
+      </c>
+      <c r="H3" s="2" t="s">
+        <v>88</v>
+      </c>
+      <c r="I3" s="2" t="s">
+        <v>89</v>
+      </c>
+      <c r="J3" s="2" t="s">
+        <v>88</v>
+      </c>
+      <c r="K3" s="2" t="s">
         <v>90</v>
       </c>
-      <c r="C3" s="2" t="s">
-        <v>91</v>
-      </c>
-      <c r="D3" s="2" t="s">
-        <v>92</v>
-      </c>
-      <c r="E3" s="2" t="s">
-        <v>93</v>
-      </c>
-      <c r="F3" s="2" t="s">
-        <v>142</v>
-      </c>
-      <c r="G3" s="2" t="s">
-        <v>94</v>
-      </c>
-      <c r="H3" s="2" t="s">
-        <v>96</v>
-      </c>
-      <c r="I3" s="2" t="s">
-        <v>97</v>
-      </c>
-      <c r="J3" s="2" t="s">
-        <v>96</v>
-      </c>
-      <c r="K3" s="2" t="s">
-        <v>99</v>
-      </c>
       <c r="L3" s="2" t="s">
-        <v>99</v>
+        <v>90</v>
       </c>
       <c r="M3" s="2" t="s">
-        <v>99</v>
-      </c>
-      <c r="N3" s="18"/>
-      <c r="O3" s="18"/>
-      <c r="P3" s="18"/>
-      <c r="Q3" s="18"/>
-      <c r="R3" s="18"/>
-      <c r="S3" s="18"/>
-      <c r="T3" s="18"/>
-      <c r="U3" s="18"/>
-      <c r="V3" s="18"/>
-      <c r="W3" s="18"/>
-      <c r="X3" s="18"/>
-      <c r="Y3" s="18"/>
-      <c r="Z3" s="18"/>
-      <c r="AA3" s="18"/>
-      <c r="AB3" s="18"/>
-      <c r="AC3" s="18"/>
+        <v>90</v>
+      </c>
+      <c r="N3" s="8"/>
+      <c r="O3" s="8"/>
+      <c r="P3" s="8"/>
+      <c r="Q3" s="8"/>
+      <c r="R3" s="8"/>
+      <c r="S3" s="8"/>
+      <c r="T3" s="8"/>
+      <c r="U3" s="8"/>
+      <c r="V3" s="8"/>
+      <c r="W3" s="8"/>
+      <c r="X3" s="8"/>
+      <c r="Y3" s="8"/>
+      <c r="Z3" s="8"/>
+      <c r="AA3" s="8"/>
+      <c r="AB3" s="8"/>
+      <c r="AC3" s="8"/>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="2" t="s">
-        <v>102</v>
+        <v>91</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>103</v>
+        <v>92</v>
       </c>
       <c r="C4" s="2" t="s">
-        <v>104</v>
+        <v>93</v>
       </c>
       <c r="D4" s="2" t="s">
-        <v>105</v>
+        <v>94</v>
       </c>
       <c r="E4" s="2" t="s">
-        <v>106</v>
+        <v>95</v>
       </c>
       <c r="F4" s="2" t="s">
-        <v>107</v>
+        <v>96</v>
       </c>
       <c r="G4" s="2" t="s">
-        <v>109</v>
+        <v>97</v>
       </c>
       <c r="H4" s="2" t="s">
-        <v>110</v>
+        <v>98</v>
       </c>
       <c r="I4" s="2" t="s">
-        <v>111</v>
+        <v>99</v>
       </c>
       <c r="J4" s="2" t="s">
         <v>49</v>
       </c>
       <c r="K4" s="2" t="s">
-        <v>137</v>
+        <v>100</v>
       </c>
       <c r="L4" s="2" t="s">
         <v>51</v>
       </c>
       <c r="M4" s="2" t="s">
-        <v>143</v>
-      </c>
-      <c r="N4" s="18"/>
-      <c r="O4" s="18"/>
-      <c r="P4" s="18"/>
-      <c r="Q4" s="18"/>
-      <c r="R4" s="18"/>
-      <c r="S4" s="18"/>
-      <c r="T4" s="18"/>
-      <c r="U4" s="18"/>
-      <c r="V4" s="18"/>
-      <c r="W4" s="18"/>
-      <c r="X4" s="18"/>
-      <c r="Y4" s="18"/>
-      <c r="Z4" s="18"/>
-      <c r="AA4" s="18"/>
-      <c r="AB4" s="18"/>
-      <c r="AC4" s="18"/>
+        <v>101</v>
+      </c>
+      <c r="N4" s="8"/>
+      <c r="O4" s="8"/>
+      <c r="P4" s="8"/>
+      <c r="Q4" s="8"/>
+      <c r="R4" s="8"/>
+      <c r="S4" s="8"/>
+      <c r="T4" s="8"/>
+      <c r="U4" s="8"/>
+      <c r="V4" s="8"/>
+      <c r="W4" s="8"/>
+      <c r="X4" s="8"/>
+      <c r="Y4" s="8"/>
+      <c r="Z4" s="8"/>
+      <c r="AA4" s="8"/>
+      <c r="AB4" s="8"/>
+      <c r="AC4" s="8"/>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="4"/>
       <c r="B5" s="2" t="s">
-        <v>117</v>
+        <v>102</v>
       </c>
       <c r="C5" s="2" t="s">
-        <v>118</v>
+        <v>103</v>
       </c>
       <c r="D5" s="2" t="s">
-        <v>119</v>
+        <v>104</v>
       </c>
       <c r="E5" s="2" t="s">
-        <v>120</v>
+        <v>105</v>
       </c>
       <c r="F5" s="2" t="s">
-        <v>94</v>
+        <v>87</v>
       </c>
       <c r="G5" s="2" t="s">
-        <v>122</v>
+        <v>106</v>
       </c>
       <c r="H5" s="2" t="s">
-        <v>123</v>
+        <v>107</v>
       </c>
       <c r="I5" s="2" t="s">
-        <v>124</v>
+        <v>108</v>
       </c>
       <c r="J5" s="2" t="s">
         <v>59</v>
       </c>
       <c r="K5" s="2" t="s">
-        <v>142</v>
+        <v>86</v>
       </c>
       <c r="L5" s="2" t="s">
-        <v>144</v>
+        <v>109</v>
       </c>
       <c r="M5" s="2" t="s">
-        <v>145</v>
-      </c>
-      <c r="N5" s="18"/>
-      <c r="O5" s="18"/>
-      <c r="P5" s="18"/>
-      <c r="Q5" s="18"/>
-      <c r="R5" s="18"/>
-      <c r="S5" s="18"/>
-      <c r="T5" s="18"/>
-      <c r="U5" s="18"/>
-      <c r="V5" s="18"/>
-      <c r="W5" s="18"/>
-      <c r="X5" s="18"/>
-      <c r="Y5" s="18"/>
-      <c r="Z5" s="18"/>
-      <c r="AA5" s="18"/>
-      <c r="AB5" s="18"/>
-      <c r="AC5" s="18"/>
+        <v>110</v>
+      </c>
+      <c r="N5" s="8"/>
+      <c r="O5" s="8"/>
+      <c r="P5" s="8"/>
+      <c r="Q5" s="8"/>
+      <c r="R5" s="8"/>
+      <c r="S5" s="8"/>
+      <c r="T5" s="8"/>
+      <c r="U5" s="8"/>
+      <c r="V5" s="8"/>
+      <c r="W5" s="8"/>
+      <c r="X5" s="8"/>
+      <c r="Y5" s="8"/>
+      <c r="Z5" s="8"/>
+      <c r="AA5" s="8"/>
+      <c r="AB5" s="8"/>
+      <c r="AC5" s="8"/>
     </row>
     <row r="6" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="4"/>
       <c r="B6" s="2" t="s">
-        <v>129</v>
+        <v>111</v>
       </c>
       <c r="C6" s="2" t="s">
-        <v>130</v>
+        <v>112</v>
       </c>
       <c r="D6" s="4"/>
       <c r="E6" s="2" t="s">
-        <v>131</v>
-      </c>
-      <c r="F6" s="19"/>
+        <v>113</v>
+      </c>
+      <c r="F6" s="10"/>
       <c r="G6" s="2" t="s">
-        <v>133</v>
+        <v>114</v>
       </c>
       <c r="H6" s="4"/>
       <c r="I6" s="4"/>
       <c r="J6" s="2" t="s">
         <v>55</v>
       </c>
-      <c r="K6" s="19"/>
+      <c r="K6" s="10"/>
       <c r="L6" s="2" t="s">
-        <v>125</v>
+        <v>115</v>
       </c>
       <c r="M6" s="2" t="s">
-        <v>112</v>
-      </c>
-      <c r="N6" s="18"/>
-      <c r="O6" s="18"/>
-      <c r="P6" s="18"/>
-      <c r="Q6" s="18"/>
-      <c r="R6" s="18"/>
-      <c r="S6" s="18"/>
-      <c r="T6" s="18"/>
-      <c r="U6" s="18"/>
-      <c r="V6" s="18"/>
-      <c r="W6" s="18"/>
-      <c r="X6" s="18"/>
-      <c r="Y6" s="18"/>
-      <c r="Z6" s="18"/>
-      <c r="AA6" s="18"/>
-      <c r="AB6" s="18"/>
-      <c r="AC6" s="18"/>
+        <v>116</v>
+      </c>
+      <c r="N6" s="8"/>
+      <c r="O6" s="8"/>
+      <c r="P6" s="8"/>
+      <c r="Q6" s="8"/>
+      <c r="R6" s="8"/>
+      <c r="S6" s="8"/>
+      <c r="T6" s="8"/>
+      <c r="U6" s="8"/>
+      <c r="V6" s="8"/>
+      <c r="W6" s="8"/>
+      <c r="X6" s="8"/>
+      <c r="Y6" s="8"/>
+      <c r="Z6" s="8"/>
+      <c r="AA6" s="8"/>
+      <c r="AB6" s="8"/>
+      <c r="AC6" s="8"/>
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="4"/>
       <c r="B7" s="4"/>
       <c r="C7" s="2" t="s">
-        <v>146</v>
+        <v>117</v>
       </c>
       <c r="D7" s="4"/>
       <c r="E7" s="2" t="s">
-        <v>147</v>
+        <v>118</v>
       </c>
       <c r="F7" s="4"/>
       <c r="G7" s="4"/>
@@ -2260,57 +1872,59 @@
       <c r="K7" s="4"/>
       <c r="L7" s="4"/>
       <c r="M7" s="4"/>
-      <c r="N7" s="18"/>
-      <c r="O7" s="18"/>
-      <c r="P7" s="18"/>
-      <c r="Q7" s="18"/>
-      <c r="R7" s="18"/>
-      <c r="S7" s="18"/>
-      <c r="T7" s="18"/>
-      <c r="U7" s="18"/>
-      <c r="V7" s="18"/>
-      <c r="W7" s="18"/>
-      <c r="X7" s="18"/>
-      <c r="Y7" s="18"/>
-      <c r="Z7" s="18"/>
-      <c r="AA7" s="18"/>
-      <c r="AB7" s="18"/>
-      <c r="AC7" s="18"/>
+      <c r="N7" s="8"/>
+      <c r="O7" s="8"/>
+      <c r="P7" s="8"/>
+      <c r="Q7" s="8"/>
+      <c r="R7" s="8"/>
+      <c r="S7" s="8"/>
+      <c r="T7" s="8"/>
+      <c r="U7" s="8"/>
+      <c r="V7" s="8"/>
+      <c r="W7" s="8"/>
+      <c r="X7" s="8"/>
+      <c r="Y7" s="8"/>
+      <c r="Z7" s="8"/>
+      <c r="AA7" s="8"/>
+      <c r="AB7" s="8"/>
+      <c r="AC7" s="8"/>
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="4"/>
       <c r="B8" s="4"/>
-      <c r="C8" s="20" t="s">
-        <v>135</v>
+      <c r="C8" s="8" t="s">
+        <v>119</v>
       </c>
       <c r="D8" s="4"/>
-      <c r="E8" s="4"/>
+      <c r="E8" s="11" t="s">
+        <v>120</v>
+      </c>
       <c r="F8" s="4"/>
       <c r="G8" s="4"/>
       <c r="H8" s="4"/>
       <c r="I8" s="4"/>
       <c r="J8" s="2" t="s">
-        <v>98</v>
+        <v>121</v>
       </c>
       <c r="K8" s="4"/>
       <c r="L8" s="4"/>
       <c r="M8" s="4"/>
-      <c r="N8" s="18"/>
-      <c r="O8" s="18"/>
-      <c r="P8" s="18"/>
-      <c r="Q8" s="18"/>
-      <c r="R8" s="18"/>
-      <c r="S8" s="18"/>
-      <c r="T8" s="18"/>
-      <c r="U8" s="18"/>
-      <c r="V8" s="18"/>
-      <c r="W8" s="18"/>
-      <c r="X8" s="18"/>
-      <c r="Y8" s="18"/>
-      <c r="Z8" s="18"/>
-      <c r="AA8" s="18"/>
-      <c r="AB8" s="18"/>
-      <c r="AC8" s="18"/>
+      <c r="N8" s="8"/>
+      <c r="O8" s="8"/>
+      <c r="P8" s="8"/>
+      <c r="Q8" s="8"/>
+      <c r="R8" s="8"/>
+      <c r="S8" s="8"/>
+      <c r="T8" s="8"/>
+      <c r="U8" s="8"/>
+      <c r="V8" s="8"/>
+      <c r="W8" s="8"/>
+      <c r="X8" s="8"/>
+      <c r="Y8" s="8"/>
+      <c r="Z8" s="8"/>
+      <c r="AA8" s="8"/>
+      <c r="AB8" s="8"/>
+      <c r="AC8" s="8"/>
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="4"/>
@@ -2326,22 +1940,22 @@
       <c r="K9" s="4"/>
       <c r="L9" s="4"/>
       <c r="M9" s="4"/>
-      <c r="N9" s="18"/>
-      <c r="O9" s="18"/>
-      <c r="P9" s="18"/>
-      <c r="Q9" s="18"/>
-      <c r="R9" s="18"/>
-      <c r="S9" s="18"/>
-      <c r="T9" s="18"/>
-      <c r="U9" s="18"/>
-      <c r="V9" s="18"/>
-      <c r="W9" s="18"/>
-      <c r="X9" s="18"/>
-      <c r="Y9" s="18"/>
-      <c r="Z9" s="18"/>
-      <c r="AA9" s="18"/>
-      <c r="AB9" s="18"/>
-      <c r="AC9" s="18"/>
+      <c r="N9" s="8"/>
+      <c r="O9" s="8"/>
+      <c r="P9" s="8"/>
+      <c r="Q9" s="8"/>
+      <c r="R9" s="8"/>
+      <c r="S9" s="8"/>
+      <c r="T9" s="8"/>
+      <c r="U9" s="8"/>
+      <c r="V9" s="8"/>
+      <c r="W9" s="8"/>
+      <c r="X9" s="8"/>
+      <c r="Y9" s="8"/>
+      <c r="Z9" s="8"/>
+      <c r="AA9" s="8"/>
+      <c r="AB9" s="8"/>
+      <c r="AC9" s="8"/>
     </row>
     <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="4"/>
@@ -2357,22 +1971,22 @@
       <c r="K10" s="4"/>
       <c r="L10" s="4"/>
       <c r="M10" s="4"/>
-      <c r="N10" s="18"/>
-      <c r="O10" s="18"/>
-      <c r="P10" s="18"/>
-      <c r="Q10" s="18"/>
-      <c r="R10" s="18"/>
-      <c r="S10" s="18"/>
-      <c r="T10" s="18"/>
-      <c r="U10" s="18"/>
-      <c r="V10" s="18"/>
-      <c r="W10" s="18"/>
-      <c r="X10" s="18"/>
-      <c r="Y10" s="18"/>
-      <c r="Z10" s="18"/>
-      <c r="AA10" s="18"/>
-      <c r="AB10" s="18"/>
-      <c r="AC10" s="18"/>
+      <c r="N10" s="8"/>
+      <c r="O10" s="8"/>
+      <c r="P10" s="8"/>
+      <c r="Q10" s="8"/>
+      <c r="R10" s="8"/>
+      <c r="S10" s="8"/>
+      <c r="T10" s="8"/>
+      <c r="U10" s="8"/>
+      <c r="V10" s="8"/>
+      <c r="W10" s="8"/>
+      <c r="X10" s="8"/>
+      <c r="Y10" s="8"/>
+      <c r="Z10" s="8"/>
+      <c r="AA10" s="8"/>
+      <c r="AB10" s="8"/>
+      <c r="AC10" s="8"/>
     </row>
     <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="4"/>
@@ -2388,22 +2002,22 @@
       <c r="K11" s="4"/>
       <c r="L11" s="4"/>
       <c r="M11" s="4"/>
-      <c r="N11" s="18"/>
-      <c r="O11" s="18"/>
-      <c r="P11" s="18"/>
-      <c r="Q11" s="18"/>
-      <c r="R11" s="18"/>
-      <c r="S11" s="18"/>
-      <c r="T11" s="18"/>
-      <c r="U11" s="18"/>
-      <c r="V11" s="18"/>
-      <c r="W11" s="18"/>
-      <c r="X11" s="18"/>
-      <c r="Y11" s="18"/>
-      <c r="Z11" s="18"/>
-      <c r="AA11" s="18"/>
-      <c r="AB11" s="18"/>
-      <c r="AC11" s="18"/>
+      <c r="N11" s="8"/>
+      <c r="O11" s="8"/>
+      <c r="P11" s="8"/>
+      <c r="Q11" s="8"/>
+      <c r="R11" s="8"/>
+      <c r="S11" s="8"/>
+      <c r="T11" s="8"/>
+      <c r="U11" s="8"/>
+      <c r="V11" s="8"/>
+      <c r="W11" s="8"/>
+      <c r="X11" s="8"/>
+      <c r="Y11" s="8"/>
+      <c r="Z11" s="8"/>
+      <c r="AA11" s="8"/>
+      <c r="AB11" s="8"/>
+      <c r="AC11" s="8"/>
     </row>
     <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="4"/>
@@ -2419,26 +2033,26 @@
       <c r="K12" s="4"/>
       <c r="L12" s="4"/>
       <c r="M12" s="4"/>
-      <c r="N12" s="18"/>
-      <c r="O12" s="18"/>
-      <c r="P12" s="18"/>
-      <c r="Q12" s="18"/>
-      <c r="R12" s="18"/>
-      <c r="S12" s="18"/>
-      <c r="T12" s="18"/>
-      <c r="U12" s="18"/>
-      <c r="V12" s="18"/>
-      <c r="W12" s="18"/>
-      <c r="X12" s="18"/>
-      <c r="Y12" s="18"/>
-      <c r="Z12" s="18"/>
-      <c r="AA12" s="18"/>
-      <c r="AB12" s="18"/>
-      <c r="AC12" s="18"/>
+      <c r="N12" s="8"/>
+      <c r="O12" s="8"/>
+      <c r="P12" s="8"/>
+      <c r="Q12" s="8"/>
+      <c r="R12" s="8"/>
+      <c r="S12" s="8"/>
+      <c r="T12" s="8"/>
+      <c r="U12" s="8"/>
+      <c r="V12" s="8"/>
+      <c r="W12" s="8"/>
+      <c r="X12" s="8"/>
+      <c r="Y12" s="8"/>
+      <c r="Z12" s="8"/>
+      <c r="AA12" s="8"/>
+      <c r="AB12" s="8"/>
+      <c r="AC12" s="8"/>
     </row>
     <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="4"/>
-      <c r="B13" s="21"/>
+      <c r="B13" s="12"/>
       <c r="C13" s="4"/>
       <c r="D13" s="4"/>
       <c r="E13" s="4"/>
@@ -2450,22 +2064,22 @@
       <c r="K13" s="4"/>
       <c r="L13" s="4"/>
       <c r="M13" s="4"/>
-      <c r="N13" s="18"/>
-      <c r="O13" s="18"/>
-      <c r="P13" s="18"/>
-      <c r="Q13" s="18"/>
-      <c r="R13" s="18"/>
-      <c r="S13" s="18"/>
-      <c r="T13" s="18"/>
-      <c r="U13" s="18"/>
-      <c r="V13" s="18"/>
-      <c r="W13" s="18"/>
-      <c r="X13" s="18"/>
-      <c r="Y13" s="18"/>
-      <c r="Z13" s="18"/>
-      <c r="AA13" s="18"/>
-      <c r="AB13" s="18"/>
-      <c r="AC13" s="18"/>
+      <c r="N13" s="8"/>
+      <c r="O13" s="8"/>
+      <c r="P13" s="8"/>
+      <c r="Q13" s="8"/>
+      <c r="R13" s="8"/>
+      <c r="S13" s="8"/>
+      <c r="T13" s="8"/>
+      <c r="U13" s="8"/>
+      <c r="V13" s="8"/>
+      <c r="W13" s="8"/>
+      <c r="X13" s="8"/>
+      <c r="Y13" s="8"/>
+      <c r="Z13" s="8"/>
+      <c r="AA13" s="8"/>
+      <c r="AB13" s="8"/>
+      <c r="AC13" s="8"/>
     </row>
     <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
     <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
@@ -3468,6 +3082,383 @@
 </worksheet>
 </file>
 
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <sheetPr filterMode="false">
+    <pageSetUpPr fitToPage="false"/>
+  </sheetPr>
+  <dimension ref="A1:Q8"/>
+  <sheetViews>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="K13" activeCellId="0" sqref="K13"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <cols>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="24.64"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="39.09"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="26.82"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="24.45"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="23.91"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="26.18"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="0" width="27.64"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="0" width="21.82"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="0" width="27.55"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="0" width="29.1"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="11" min="11" style="0" width="61.92"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="12" min="12" style="0" width="33.37"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="13" min="13" style="0" width="31.82"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="14" min="14" style="0" width="45.01"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="15" min="15" style="0" width="26.55"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="16" min="16" style="0" width="30.36"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="17" min="17" style="0" width="38.1"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="18" min="18" style="0" width="31.69"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="19" min="19" style="0" width="36.31"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="21" min="20" style="0" width="27.12"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="22" min="22" style="0" width="20.14"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="23" min="23" style="0" width="36.57"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="24" min="24" style="0" width="19.71"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="25" min="25" style="0" width="36.71"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="26" style="0" width="14.43"/>
+  </cols>
+  <sheetData>
+    <row r="1" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1" s="7" t="s">
+        <v>66</v>
+      </c>
+      <c r="B1" s="7" t="s">
+        <v>67</v>
+      </c>
+      <c r="C1" s="7" t="s">
+        <v>68</v>
+      </c>
+      <c r="D1" s="7" t="s">
+        <v>69</v>
+      </c>
+      <c r="E1" s="7" t="s">
+        <v>70</v>
+      </c>
+      <c r="F1" s="7" t="s">
+        <v>71</v>
+      </c>
+      <c r="G1" s="7" t="s">
+        <v>122</v>
+      </c>
+      <c r="H1" s="7" t="s">
+        <v>28</v>
+      </c>
+      <c r="I1" s="7" t="s">
+        <v>72</v>
+      </c>
+      <c r="J1" s="7" t="s">
+        <v>23</v>
+      </c>
+      <c r="K1" s="13" t="s">
+        <v>29</v>
+      </c>
+      <c r="L1" s="7" t="s">
+        <v>26</v>
+      </c>
+      <c r="M1" s="7" t="s">
+        <v>27</v>
+      </c>
+      <c r="N1" s="14" t="s">
+        <v>123</v>
+      </c>
+      <c r="O1" s="1" t="s">
+        <v>124</v>
+      </c>
+      <c r="P1" s="15" t="s">
+        <v>125</v>
+      </c>
+      <c r="Q1" s="15" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A2" s="2" t="s">
+        <v>74</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>75</v>
+      </c>
+      <c r="C2" s="2" t="s">
+        <v>76</v>
+      </c>
+      <c r="D2" s="2" t="s">
+        <v>77</v>
+      </c>
+      <c r="E2" s="2" t="s">
+        <v>78</v>
+      </c>
+      <c r="F2" s="9" t="s">
+        <v>79</v>
+      </c>
+      <c r="G2" s="2" t="s">
+        <v>127</v>
+      </c>
+      <c r="H2" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="I2" s="2" t="s">
+        <v>80</v>
+      </c>
+      <c r="J2" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="K2" s="16" t="s">
+        <v>39</v>
+      </c>
+      <c r="L2" s="2" t="s">
+        <v>36</v>
+      </c>
+      <c r="M2" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="N2" s="16" t="s">
+        <v>128</v>
+      </c>
+      <c r="O2" s="2" t="s">
+        <v>129</v>
+      </c>
+      <c r="P2" s="17" t="s">
+        <v>130</v>
+      </c>
+      <c r="Q2" s="17" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A3" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="B3" s="2" t="s">
+        <v>82</v>
+      </c>
+      <c r="C3" s="2" t="s">
+        <v>83</v>
+      </c>
+      <c r="D3" s="2" t="s">
+        <v>84</v>
+      </c>
+      <c r="E3" s="2" t="s">
+        <v>85</v>
+      </c>
+      <c r="F3" s="2" t="s">
+        <v>87</v>
+      </c>
+      <c r="G3" s="2" t="s">
+        <v>132</v>
+      </c>
+      <c r="H3" s="2" t="s">
+        <v>87</v>
+      </c>
+      <c r="I3" s="2" t="s">
+        <v>88</v>
+      </c>
+      <c r="J3" s="2" t="s">
+        <v>89</v>
+      </c>
+      <c r="K3" s="16" t="s">
+        <v>121</v>
+      </c>
+      <c r="L3" s="2" t="s">
+        <v>90</v>
+      </c>
+      <c r="M3" s="2" t="s">
+        <v>90</v>
+      </c>
+      <c r="N3" s="16" t="s">
+        <v>133</v>
+      </c>
+      <c r="O3" s="2" t="s">
+        <v>90</v>
+      </c>
+      <c r="P3" s="17" t="s">
+        <v>134</v>
+      </c>
+      <c r="Q3" s="17" t="s">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="4" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A4" s="2" t="s">
+        <v>91</v>
+      </c>
+      <c r="B4" s="2" t="s">
+        <v>92</v>
+      </c>
+      <c r="C4" s="2" t="s">
+        <v>93</v>
+      </c>
+      <c r="D4" s="2" t="s">
+        <v>94</v>
+      </c>
+      <c r="E4" s="2" t="s">
+        <v>95</v>
+      </c>
+      <c r="F4" s="2" t="s">
+        <v>96</v>
+      </c>
+      <c r="G4" s="2" t="s">
+        <v>135</v>
+      </c>
+      <c r="H4" s="2" t="s">
+        <v>97</v>
+      </c>
+      <c r="I4" s="2" t="s">
+        <v>98</v>
+      </c>
+      <c r="J4" s="2" t="s">
+        <v>99</v>
+      </c>
+      <c r="K4" s="2" t="s">
+        <v>88</v>
+      </c>
+      <c r="L4" s="2" t="s">
+        <v>51</v>
+      </c>
+      <c r="M4" s="2" t="s">
+        <v>116</v>
+      </c>
+      <c r="N4" s="2" t="s">
+        <v>136</v>
+      </c>
+      <c r="O4" s="2" t="s">
+        <v>137</v>
+      </c>
+      <c r="P4" s="17" t="s">
+        <v>138</v>
+      </c>
+      <c r="Q4" s="17" t="s">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="5" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A5" s="2"/>
+      <c r="B5" s="2" t="s">
+        <v>102</v>
+      </c>
+      <c r="C5" s="2" t="s">
+        <v>103</v>
+      </c>
+      <c r="D5" s="2" t="s">
+        <v>104</v>
+      </c>
+      <c r="E5" s="2" t="s">
+        <v>105</v>
+      </c>
+      <c r="F5" s="2"/>
+      <c r="G5" s="3" t="s">
+        <v>140</v>
+      </c>
+      <c r="H5" s="2" t="s">
+        <v>106</v>
+      </c>
+      <c r="I5" s="2" t="s">
+        <v>107</v>
+      </c>
+      <c r="J5" s="2" t="s">
+        <v>108</v>
+      </c>
+      <c r="K5" s="2" t="s">
+        <v>49</v>
+      </c>
+      <c r="L5" s="2" t="s">
+        <v>115</v>
+      </c>
+      <c r="M5" s="2"/>
+      <c r="N5" s="2" t="s">
+        <v>141</v>
+      </c>
+      <c r="O5" s="2" t="s">
+        <v>142</v>
+      </c>
+      <c r="P5" s="2" t="s">
+        <v>143</v>
+      </c>
+      <c r="Q5" s="18"/>
+    </row>
+    <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A6" s="2"/>
+      <c r="B6" s="2" t="s">
+        <v>111</v>
+      </c>
+      <c r="C6" s="2" t="s">
+        <v>112</v>
+      </c>
+      <c r="D6" s="2"/>
+      <c r="E6" s="2" t="s">
+        <v>113</v>
+      </c>
+      <c r="F6" s="2"/>
+      <c r="G6" s="2" t="s">
+        <v>144</v>
+      </c>
+      <c r="H6" s="2" t="s">
+        <v>114</v>
+      </c>
+      <c r="I6" s="2"/>
+      <c r="J6" s="2"/>
+      <c r="K6" s="2" t="s">
+        <v>59</v>
+      </c>
+      <c r="L6" s="2"/>
+      <c r="M6" s="2"/>
+      <c r="N6" s="2" t="s">
+        <v>145</v>
+      </c>
+      <c r="O6" s="2"/>
+      <c r="P6" s="2"/>
+      <c r="Q6" s="2"/>
+    </row>
+    <row r="7" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C7" s="2" t="s">
+        <v>119</v>
+      </c>
+      <c r="G7" s="2" t="s">
+        <v>146</v>
+      </c>
+      <c r="K7" s="2" t="s">
+        <v>55</v>
+      </c>
+      <c r="N7" s="2" t="s">
+        <v>100</v>
+      </c>
+      <c r="O7" s="2"/>
+      <c r="P7" s="19"/>
+      <c r="Q7" s="19"/>
+    </row>
+    <row r="8" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="G8" s="2" t="s">
+        <v>147</v>
+      </c>
+      <c r="K8" s="2" t="s">
+        <v>61</v>
+      </c>
+      <c r="N8" s="2" t="s">
+        <v>148</v>
+      </c>
+      <c r="O8" s="2"/>
+      <c r="P8" s="19"/>
+      <c r="Q8" s="19"/>
+    </row>
+  </sheetData>
+  <conditionalFormatting sqref="G2:G7 K8 N8">
+    <cfRule type="expression" priority="2" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="0">
+      <formula>LEN(TRIM(#ref!))&gt;0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
+  <pageMargins left="0.747916666666667" right="0.747916666666667" top="0.984027777777778" bottom="0.984027777777778" header="0.511805555555555" footer="0.511805555555555"/>
+  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <headerFooter differentFirst="false" differentOddEven="false">
+    <oddHeader/>
+    <oddFooter/>
+  </headerFooter>
+</worksheet>
+</file>
+
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <sheetPr filterMode="false">
@@ -3496,7 +3487,7 @@
   <sheetData>
     <row r="1" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="7" t="s">
-        <v>148</v>
+        <v>149</v>
       </c>
       <c r="B1" s="7" t="s">
         <v>28</v>
@@ -3504,38 +3495,38 @@
       <c r="C1" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="D1" s="22" t="s">
+      <c r="D1" s="20" t="s">
         <v>29</v>
       </c>
       <c r="E1" s="7" t="s">
-        <v>75</v>
+        <v>124</v>
       </c>
       <c r="F1" s="7" t="s">
-        <v>140</v>
-      </c>
-      <c r="G1" s="23" t="s">
+        <v>73</v>
+      </c>
+      <c r="G1" s="21" t="s">
         <v>26</v>
       </c>
-      <c r="H1" s="23" t="s">
-        <v>76</v>
-      </c>
-      <c r="I1" s="23" t="s">
+      <c r="H1" s="21" t="s">
+        <v>125</v>
+      </c>
+      <c r="I1" s="21" t="s">
         <v>27</v>
       </c>
-      <c r="J1" s="23" t="s">
-        <v>77</v>
-      </c>
-      <c r="K1" s="18"/>
-      <c r="L1" s="18"/>
-      <c r="M1" s="18"/>
-      <c r="N1" s="18"/>
-      <c r="O1" s="18"/>
-      <c r="P1" s="18"/>
-      <c r="Q1" s="18"/>
+      <c r="J1" s="21" t="s">
+        <v>126</v>
+      </c>
+      <c r="K1" s="8"/>
+      <c r="L1" s="8"/>
+      <c r="M1" s="8"/>
+      <c r="N1" s="8"/>
+      <c r="O1" s="8"/>
+      <c r="P1" s="8"/>
+      <c r="Q1" s="8"/>
     </row>
     <row r="2" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="2" t="s">
-        <v>149</v>
+        <v>150</v>
       </c>
       <c r="B2" s="2" t="s">
         <v>38</v>
@@ -3543,307 +3534,307 @@
       <c r="C2" s="2" t="s">
         <v>33</v>
       </c>
-      <c r="D2" s="12" t="s">
+      <c r="D2" s="16" t="s">
         <v>39</v>
       </c>
       <c r="E2" s="2" t="s">
-        <v>87</v>
+        <v>129</v>
       </c>
       <c r="F2" s="2" t="s">
-        <v>150</v>
-      </c>
-      <c r="G2" s="13" t="s">
+        <v>151</v>
+      </c>
+      <c r="G2" s="17" t="s">
         <v>36</v>
       </c>
-      <c r="H2" s="13" t="s">
-        <v>88</v>
-      </c>
-      <c r="I2" s="13" t="s">
+      <c r="H2" s="17" t="s">
+        <v>130</v>
+      </c>
+      <c r="I2" s="17" t="s">
         <v>37</v>
       </c>
-      <c r="J2" s="13" t="s">
-        <v>89</v>
-      </c>
-      <c r="K2" s="18"/>
-      <c r="L2" s="18"/>
-      <c r="M2" s="18"/>
-      <c r="N2" s="18"/>
-      <c r="O2" s="18"/>
-      <c r="P2" s="18"/>
-      <c r="Q2" s="18"/>
+      <c r="J2" s="17" t="s">
+        <v>131</v>
+      </c>
+      <c r="K2" s="8"/>
+      <c r="L2" s="8"/>
+      <c r="M2" s="8"/>
+      <c r="N2" s="8"/>
+      <c r="O2" s="8"/>
+      <c r="P2" s="8"/>
+      <c r="Q2" s="8"/>
     </row>
     <row r="3" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="4"/>
       <c r="B3" s="2" t="s">
-        <v>109</v>
+        <v>97</v>
       </c>
       <c r="C3" s="2" t="s">
         <v>42</v>
       </c>
-      <c r="D3" s="12" t="s">
+      <c r="D3" s="16" t="s">
         <v>43</v>
       </c>
       <c r="E3" s="2" t="s">
-        <v>99</v>
+        <v>90</v>
       </c>
       <c r="F3" s="2" t="s">
-        <v>151</v>
-      </c>
-      <c r="G3" s="13" t="s">
         <v>152</v>
       </c>
-      <c r="H3" s="13" t="s">
-        <v>101</v>
-      </c>
-      <c r="I3" s="13" t="s">
-        <v>152</v>
-      </c>
-      <c r="J3" s="13" t="s">
-        <v>101</v>
-      </c>
-      <c r="K3" s="18"/>
-      <c r="L3" s="18"/>
-      <c r="M3" s="18"/>
-      <c r="N3" s="18"/>
-      <c r="O3" s="18"/>
-      <c r="P3" s="18"/>
-      <c r="Q3" s="18"/>
+      <c r="G3" s="17" t="s">
+        <v>153</v>
+      </c>
+      <c r="H3" s="17" t="s">
+        <v>134</v>
+      </c>
+      <c r="I3" s="17" t="s">
+        <v>153</v>
+      </c>
+      <c r="J3" s="17" t="s">
+        <v>134</v>
+      </c>
+      <c r="K3" s="8"/>
+      <c r="L3" s="8"/>
+      <c r="M3" s="8"/>
+      <c r="N3" s="8"/>
+      <c r="O3" s="8"/>
+      <c r="P3" s="8"/>
+      <c r="Q3" s="8"/>
     </row>
     <row r="4" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="4"/>
-      <c r="B4" s="11" t="s">
-        <v>122</v>
+      <c r="B4" s="9" t="s">
+        <v>106</v>
       </c>
       <c r="C4" s="2" t="s">
         <v>48</v>
       </c>
-      <c r="D4" s="12" t="s">
+      <c r="D4" s="16" t="s">
         <v>49</v>
       </c>
       <c r="E4" s="2" t="s">
+        <v>86</v>
+      </c>
+      <c r="F4" s="2" t="s">
+        <v>86</v>
+      </c>
+      <c r="G4" s="17" t="s">
+        <v>51</v>
+      </c>
+      <c r="H4" s="17" t="s">
+        <v>138</v>
+      </c>
+      <c r="I4" s="17" t="s">
+        <v>52</v>
+      </c>
+      <c r="J4" s="17" t="s">
+        <v>138</v>
+      </c>
+      <c r="K4" s="8"/>
+      <c r="L4" s="8"/>
+      <c r="M4" s="8"/>
+      <c r="N4" s="8"/>
+      <c r="O4" s="8"/>
+      <c r="P4" s="8"/>
+      <c r="Q4" s="8"/>
+    </row>
+    <row r="5" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A5" s="22"/>
+      <c r="B5" s="2" t="s">
+        <v>114</v>
+      </c>
+      <c r="C5" s="2" t="s">
+        <v>154</v>
+      </c>
+      <c r="D5" s="16" t="s">
+        <v>55</v>
+      </c>
+      <c r="E5" s="2" t="s">
         <v>142</v>
       </c>
-      <c r="F4" s="2" t="s">
-        <v>142</v>
-      </c>
-      <c r="G4" s="13" t="s">
-        <v>51</v>
-      </c>
-      <c r="H4" s="13" t="s">
-        <v>115</v>
-      </c>
-      <c r="I4" s="13" t="s">
-        <v>52</v>
-      </c>
-      <c r="J4" s="13" t="s">
-        <v>115</v>
-      </c>
-      <c r="K4" s="18"/>
-      <c r="L4" s="18"/>
-      <c r="M4" s="18"/>
-      <c r="N4" s="18"/>
-      <c r="O4" s="18"/>
-      <c r="P4" s="18"/>
-      <c r="Q4" s="18"/>
-    </row>
-    <row r="5" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="24"/>
-      <c r="B5" s="2" t="s">
-        <v>133</v>
-      </c>
-      <c r="C5" s="2" t="s">
-        <v>153</v>
-      </c>
-      <c r="D5" s="12" t="s">
-        <v>55</v>
-      </c>
-      <c r="E5" s="2" t="s">
-        <v>127</v>
-      </c>
       <c r="F5" s="2" t="s">
-        <v>154</v>
-      </c>
-      <c r="G5" s="13" t="s">
+        <v>155</v>
+      </c>
+      <c r="G5" s="17" t="s">
         <v>57</v>
       </c>
       <c r="H5" s="2" t="s">
-        <v>128</v>
-      </c>
-      <c r="I5" s="13" t="s">
+        <v>143</v>
+      </c>
+      <c r="I5" s="17" t="s">
         <v>58</v>
       </c>
       <c r="J5" s="2" t="s">
-        <v>116</v>
-      </c>
-      <c r="K5" s="18"/>
-      <c r="L5" s="18"/>
-      <c r="M5" s="18"/>
-      <c r="N5" s="18"/>
-      <c r="O5" s="18"/>
-      <c r="P5" s="18"/>
-      <c r="Q5" s="18"/>
+        <v>139</v>
+      </c>
+      <c r="K5" s="8"/>
+      <c r="L5" s="8"/>
+      <c r="M5" s="8"/>
+      <c r="N5" s="8"/>
+      <c r="O5" s="8"/>
+      <c r="P5" s="8"/>
+      <c r="Q5" s="8"/>
     </row>
     <row r="6" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A6" s="25"/>
+      <c r="A6" s="23"/>
       <c r="B6" s="4"/>
       <c r="C6" s="4"/>
-      <c r="D6" s="12" t="s">
+      <c r="D6" s="16" t="s">
         <v>59</v>
       </c>
-      <c r="E6" s="25"/>
-      <c r="F6" s="25"/>
+      <c r="E6" s="23"/>
+      <c r="F6" s="23"/>
       <c r="G6" s="2" t="s">
-        <v>125</v>
-      </c>
-      <c r="H6" s="26"/>
+        <v>115</v>
+      </c>
+      <c r="H6" s="24"/>
       <c r="I6" s="2" t="s">
-        <v>112</v>
-      </c>
-      <c r="J6" s="27"/>
-      <c r="K6" s="18"/>
-      <c r="L6" s="18"/>
-      <c r="M6" s="18"/>
-      <c r="N6" s="18"/>
-      <c r="O6" s="18"/>
-      <c r="P6" s="18"/>
-      <c r="Q6" s="18"/>
+        <v>116</v>
+      </c>
+      <c r="J6" s="25"/>
+      <c r="K6" s="8"/>
+      <c r="L6" s="8"/>
+      <c r="M6" s="8"/>
+      <c r="N6" s="8"/>
+      <c r="O6" s="8"/>
+      <c r="P6" s="8"/>
+      <c r="Q6" s="8"/>
     </row>
     <row r="7" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A7" s="25"/>
+      <c r="A7" s="23"/>
       <c r="B7" s="4"/>
       <c r="C7" s="4"/>
-      <c r="D7" s="12" t="s">
+      <c r="D7" s="16" t="s">
         <v>61</v>
       </c>
-      <c r="E7" s="25"/>
-      <c r="F7" s="25"/>
-      <c r="G7" s="27"/>
-      <c r="H7" s="27"/>
-      <c r="I7" s="27"/>
-      <c r="J7" s="27"/>
-      <c r="K7" s="18"/>
-      <c r="L7" s="18"/>
-      <c r="M7" s="18"/>
-      <c r="N7" s="18"/>
-      <c r="O7" s="18"/>
-      <c r="P7" s="18"/>
-      <c r="Q7" s="18"/>
+      <c r="E7" s="23"/>
+      <c r="F7" s="23"/>
+      <c r="G7" s="25"/>
+      <c r="H7" s="25"/>
+      <c r="I7" s="25"/>
+      <c r="J7" s="25"/>
+      <c r="K7" s="8"/>
+      <c r="L7" s="8"/>
+      <c r="M7" s="8"/>
+      <c r="N7" s="8"/>
+      <c r="O7" s="8"/>
+      <c r="P7" s="8"/>
+      <c r="Q7" s="8"/>
     </row>
     <row r="8" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A8" s="25"/>
+      <c r="A8" s="23"/>
       <c r="B8" s="4"/>
       <c r="C8" s="4"/>
       <c r="D8" s="2" t="s">
-        <v>96</v>
+        <v>88</v>
       </c>
       <c r="E8" s="4"/>
       <c r="F8" s="4"/>
-      <c r="G8" s="27"/>
-      <c r="H8" s="27"/>
-      <c r="I8" s="27"/>
-      <c r="J8" s="27"/>
-      <c r="K8" s="18"/>
-      <c r="L8" s="18"/>
-      <c r="M8" s="18"/>
-      <c r="N8" s="18"/>
-      <c r="O8" s="18"/>
-      <c r="P8" s="18"/>
-      <c r="Q8" s="18"/>
+      <c r="G8" s="25"/>
+      <c r="H8" s="25"/>
+      <c r="I8" s="25"/>
+      <c r="J8" s="25"/>
+      <c r="K8" s="8"/>
+      <c r="L8" s="8"/>
+      <c r="M8" s="8"/>
+      <c r="N8" s="8"/>
+      <c r="O8" s="8"/>
+      <c r="P8" s="8"/>
+      <c r="Q8" s="8"/>
     </row>
     <row r="9" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="4"/>
       <c r="B9" s="4"/>
       <c r="C9" s="4"/>
-      <c r="D9" s="28"/>
+      <c r="D9" s="26"/>
       <c r="E9" s="4"/>
       <c r="F9" s="4"/>
-      <c r="G9" s="27"/>
-      <c r="H9" s="27"/>
-      <c r="I9" s="27"/>
-      <c r="J9" s="27"/>
-      <c r="K9" s="18"/>
-      <c r="L9" s="18"/>
-      <c r="M9" s="18"/>
-      <c r="N9" s="18"/>
-      <c r="O9" s="18"/>
-      <c r="P9" s="18"/>
-      <c r="Q9" s="18"/>
+      <c r="G9" s="25"/>
+      <c r="H9" s="25"/>
+      <c r="I9" s="25"/>
+      <c r="J9" s="25"/>
+      <c r="K9" s="8"/>
+      <c r="L9" s="8"/>
+      <c r="M9" s="8"/>
+      <c r="N9" s="8"/>
+      <c r="O9" s="8"/>
+      <c r="P9" s="8"/>
+      <c r="Q9" s="8"/>
     </row>
     <row r="10" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="4"/>
       <c r="B10" s="4"/>
       <c r="C10" s="4"/>
-      <c r="D10" s="28"/>
+      <c r="D10" s="26"/>
       <c r="E10" s="4"/>
       <c r="F10" s="4"/>
-      <c r="G10" s="27"/>
-      <c r="H10" s="27"/>
-      <c r="I10" s="27"/>
-      <c r="J10" s="27"/>
-      <c r="K10" s="18"/>
-      <c r="L10" s="18"/>
-      <c r="M10" s="18"/>
-      <c r="N10" s="18"/>
-      <c r="O10" s="18"/>
-      <c r="P10" s="18"/>
-      <c r="Q10" s="18"/>
+      <c r="G10" s="25"/>
+      <c r="H10" s="25"/>
+      <c r="I10" s="25"/>
+      <c r="J10" s="25"/>
+      <c r="K10" s="8"/>
+      <c r="L10" s="8"/>
+      <c r="M10" s="8"/>
+      <c r="N10" s="8"/>
+      <c r="O10" s="8"/>
+      <c r="P10" s="8"/>
+      <c r="Q10" s="8"/>
     </row>
     <row r="11" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="4"/>
       <c r="B11" s="4"/>
       <c r="C11" s="4"/>
-      <c r="D11" s="28"/>
+      <c r="D11" s="26"/>
       <c r="E11" s="4"/>
       <c r="F11" s="4"/>
-      <c r="G11" s="27"/>
-      <c r="H11" s="27"/>
-      <c r="I11" s="27"/>
-      <c r="J11" s="27"/>
-      <c r="K11" s="18"/>
-      <c r="L11" s="18"/>
-      <c r="M11" s="18"/>
-      <c r="N11" s="18"/>
-      <c r="O11" s="18"/>
-      <c r="P11" s="18"/>
-      <c r="Q11" s="18"/>
+      <c r="G11" s="25"/>
+      <c r="H11" s="25"/>
+      <c r="I11" s="25"/>
+      <c r="J11" s="25"/>
+      <c r="K11" s="8"/>
+      <c r="L11" s="8"/>
+      <c r="M11" s="8"/>
+      <c r="N11" s="8"/>
+      <c r="O11" s="8"/>
+      <c r="P11" s="8"/>
+      <c r="Q11" s="8"/>
     </row>
     <row r="12" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="4"/>
       <c r="B12" s="4"/>
       <c r="C12" s="4"/>
-      <c r="D12" s="29"/>
+      <c r="D12" s="27"/>
       <c r="E12" s="4"/>
       <c r="F12" s="4"/>
-      <c r="G12" s="27"/>
-      <c r="H12" s="27"/>
-      <c r="I12" s="27"/>
-      <c r="J12" s="27"/>
-      <c r="K12" s="18"/>
-      <c r="L12" s="18"/>
-      <c r="M12" s="18"/>
-      <c r="N12" s="18"/>
-      <c r="O12" s="18"/>
-      <c r="P12" s="18"/>
-      <c r="Q12" s="18"/>
+      <c r="G12" s="25"/>
+      <c r="H12" s="25"/>
+      <c r="I12" s="25"/>
+      <c r="J12" s="25"/>
+      <c r="K12" s="8"/>
+      <c r="L12" s="8"/>
+      <c r="M12" s="8"/>
+      <c r="N12" s="8"/>
+      <c r="O12" s="8"/>
+      <c r="P12" s="8"/>
+      <c r="Q12" s="8"/>
     </row>
     <row r="13" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="4"/>
       <c r="B13" s="4"/>
       <c r="C13" s="4"/>
-      <c r="D13" s="29"/>
+      <c r="D13" s="27"/>
       <c r="E13" s="4"/>
       <c r="F13" s="4"/>
-      <c r="G13" s="27"/>
-      <c r="H13" s="27"/>
-      <c r="I13" s="27"/>
-      <c r="J13" s="27"/>
-      <c r="K13" s="18"/>
-      <c r="L13" s="18"/>
-      <c r="M13" s="18"/>
-      <c r="N13" s="18"/>
-      <c r="O13" s="18"/>
-      <c r="P13" s="18"/>
-      <c r="Q13" s="18"/>
+      <c r="G13" s="25"/>
+      <c r="H13" s="25"/>
+      <c r="I13" s="25"/>
+      <c r="J13" s="25"/>
+      <c r="K13" s="8"/>
+      <c r="L13" s="8"/>
+      <c r="M13" s="8"/>
+      <c r="N13" s="8"/>
+      <c r="O13" s="8"/>
+      <c r="P13" s="8"/>
+      <c r="Q13" s="8"/>
     </row>
     <row r="1048576" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
   </sheetData>

</xml_diff>

<commit_message>
Adding extra attributes in examineeBatch Table
</commit_message>
<xml_diff>
--- a/OAES Database Design.xlsx
+++ b/OAES Database Design.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="2"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="OAES_USER_MGMT" sheetId="1" state="visible" r:id="rId2"/>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="299" uniqueCount="156">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="302" uniqueCount="159">
   <si>
     <t xml:space="preserve">oaes_user</t>
   </si>
@@ -434,7 +434,7 @@
     <t xml:space="preserve">invigilator_email</t>
   </si>
   <si>
-    <t xml:space="preserve">status (NOT_Started, IN_Progress,Completed,Abandoned )</t>
+    <t xml:space="preserve">status (IN_Progress,Completed,Abandoned)</t>
   </si>
   <si>
     <t xml:space="preserve">attempt_id FK refers ATTEMPT</t>
@@ -446,6 +446,9 @@
     <t xml:space="preserve">response_true_false_code UNIQUE NOTNULL</t>
   </si>
   <si>
+    <t xml:space="preserve">examinee_batch_start_time</t>
+  </si>
+  <si>
     <t xml:space="preserve">invigilator_password</t>
   </si>
   <si>
@@ -458,10 +461,16 @@
     <t xml:space="preserve">response_mcq_code UNIQUE NOTNULL</t>
   </si>
   <si>
+    <t xml:space="preserve">examinee_batch_end_time</t>
+  </si>
+  <si>
     <t xml:space="preserve">batch_id FK refers BATCH_COURSE</t>
   </si>
   <si>
     <t xml:space="preserve">attempt_end_time</t>
+  </si>
+  <si>
+    <t xml:space="preserve">examinee_batch_status(NOT_Started, IN_Progress,Completed)</t>
   </si>
   <si>
     <t xml:space="preserve">user_status(Active, NOT_Active)</t>
@@ -501,7 +510,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="General"/>
   </numFmts>
-  <fonts count="11">
+  <fonts count="12">
     <font>
       <sz val="10"/>
       <color rgb="FF000000"/>
@@ -560,6 +569,12 @@
       <name val="Calibri"/>
       <family val="0"/>
       <charset val="1"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="0"/>
     </font>
     <font>
       <sz val="11"/>
@@ -721,10 +736,6 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
     <xf numFmtId="164" fontId="5" fillId="4" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -749,7 +760,11 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="9" fillId="0" borderId="4" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="9" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="10" fillId="0" borderId="4" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -765,7 +780,7 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="10" fillId="4" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="11" fillId="4" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -791,12 +806,12 @@
     </xf>
   </cellXfs>
   <cellStyles count="6">
-    <cellStyle name="Normal" xfId="0" builtinId="0" customBuiltin="false"/>
-    <cellStyle name="Comma" xfId="15" builtinId="3" customBuiltin="false"/>
-    <cellStyle name="Comma [0]" xfId="16" builtinId="6" customBuiltin="false"/>
-    <cellStyle name="Currency" xfId="17" builtinId="4" customBuiltin="false"/>
-    <cellStyle name="Currency [0]" xfId="18" builtinId="7" customBuiltin="false"/>
-    <cellStyle name="Percent" xfId="19" builtinId="5" customBuiltin="false"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Comma" xfId="15" builtinId="3"/>
+    <cellStyle name="Comma [0]" xfId="16" builtinId="6"/>
+    <cellStyle name="Currency" xfId="17" builtinId="4"/>
+    <cellStyle name="Currency [0]" xfId="18" builtinId="7"/>
+    <cellStyle name="Percent" xfId="19" builtinId="5"/>
   </cellStyles>
   <dxfs count="1">
     <dxf>
@@ -1499,9 +1514,9 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:AC14"/>
+  <dimension ref="A1:AC998"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="D1" colorId="64" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="D1" colorId="64" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="E17" activeCellId="0" sqref="E17"/>
     </sheetView>
   </sheetViews>
@@ -1896,7 +1911,7 @@
         <v>119</v>
       </c>
       <c r="D8" s="4"/>
-      <c r="E8" s="11" t="s">
+      <c r="E8" s="2" t="s">
         <v>120</v>
       </c>
       <c r="F8" s="4"/>
@@ -2052,7 +2067,7 @@
     </row>
     <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="4"/>
-      <c r="B13" s="12"/>
+      <c r="B13" s="11"/>
       <c r="C13" s="4"/>
       <c r="D13" s="4"/>
       <c r="E13" s="4"/>
@@ -3089,8 +3104,8 @@
   </sheetPr>
   <dimension ref="A1:Q8"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="K13" activeCellId="0" sqref="K13"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="J1" colorId="64" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="F10" activeCellId="0" sqref="F10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -3100,7 +3115,7 @@
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="26.82"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="24.45"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="23.91"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="26.18"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="48.01"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="0" width="27.64"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="0" width="21.82"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="0" width="27.55"/>
@@ -3108,7 +3123,7 @@
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="11" min="11" style="0" width="61.92"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="12" min="12" style="0" width="33.37"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="13" min="13" style="0" width="31.82"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="14" min="14" style="0" width="45.01"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="14" min="14" style="0" width="36.91"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="15" min="15" style="0" width="26.55"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="16" min="16" style="0" width="30.36"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="17" min="17" style="0" width="38.1"/>
@@ -3153,7 +3168,7 @@
       <c r="J1" s="7" t="s">
         <v>23</v>
       </c>
-      <c r="K1" s="13" t="s">
+      <c r="K1" s="12" t="s">
         <v>29</v>
       </c>
       <c r="L1" s="7" t="s">
@@ -3162,16 +3177,16 @@
       <c r="M1" s="7" t="s">
         <v>27</v>
       </c>
-      <c r="N1" s="14" t="s">
+      <c r="N1" s="13" t="s">
         <v>123</v>
       </c>
       <c r="O1" s="1" t="s">
         <v>124</v>
       </c>
-      <c r="P1" s="15" t="s">
+      <c r="P1" s="14" t="s">
         <v>125</v>
       </c>
-      <c r="Q1" s="15" t="s">
+      <c r="Q1" s="14" t="s">
         <v>126</v>
       </c>
     </row>
@@ -3206,7 +3221,7 @@
       <c r="J2" s="2" t="s">
         <v>33</v>
       </c>
-      <c r="K2" s="16" t="s">
+      <c r="K2" s="15" t="s">
         <v>39</v>
       </c>
       <c r="L2" s="2" t="s">
@@ -3215,16 +3230,16 @@
       <c r="M2" s="2" t="s">
         <v>37</v>
       </c>
-      <c r="N2" s="16" t="s">
+      <c r="N2" s="15" t="s">
         <v>128</v>
       </c>
       <c r="O2" s="2" t="s">
         <v>129</v>
       </c>
-      <c r="P2" s="17" t="s">
+      <c r="P2" s="16" t="s">
         <v>130</v>
       </c>
-      <c r="Q2" s="17" t="s">
+      <c r="Q2" s="16" t="s">
         <v>131</v>
       </c>
     </row>
@@ -3259,7 +3274,7 @@
       <c r="J3" s="2" t="s">
         <v>89</v>
       </c>
-      <c r="K3" s="16" t="s">
+      <c r="K3" s="15" t="s">
         <v>121</v>
       </c>
       <c r="L3" s="2" t="s">
@@ -3268,16 +3283,16 @@
       <c r="M3" s="2" t="s">
         <v>90</v>
       </c>
-      <c r="N3" s="16" t="s">
+      <c r="N3" s="15" t="s">
         <v>133</v>
       </c>
       <c r="O3" s="2" t="s">
         <v>90</v>
       </c>
-      <c r="P3" s="17" t="s">
+      <c r="P3" s="16" t="s">
         <v>134</v>
       </c>
-      <c r="Q3" s="17" t="s">
+      <c r="Q3" s="16" t="s">
         <v>134</v>
       </c>
     </row>
@@ -3327,10 +3342,10 @@
       <c r="O4" s="2" t="s">
         <v>137</v>
       </c>
-      <c r="P4" s="17" t="s">
+      <c r="P4" s="16" t="s">
         <v>138</v>
       </c>
-      <c r="Q4" s="17" t="s">
+      <c r="Q4" s="16" t="s">
         <v>139</v>
       </c>
     </row>
@@ -3348,9 +3363,11 @@
       <c r="E5" s="2" t="s">
         <v>105</v>
       </c>
-      <c r="F5" s="2"/>
+      <c r="F5" s="17" t="s">
+        <v>140</v>
+      </c>
       <c r="G5" s="3" t="s">
-        <v>140</v>
+        <v>141</v>
       </c>
       <c r="H5" s="2" t="s">
         <v>106</v>
@@ -3369,13 +3386,13 @@
       </c>
       <c r="M5" s="2"/>
       <c r="N5" s="2" t="s">
-        <v>141</v>
+        <v>142</v>
       </c>
       <c r="O5" s="2" t="s">
-        <v>142</v>
+        <v>143</v>
       </c>
       <c r="P5" s="2" t="s">
-        <v>143</v>
+        <v>144</v>
       </c>
       <c r="Q5" s="18"/>
     </row>
@@ -3391,9 +3408,11 @@
       <c r="E6" s="2" t="s">
         <v>113</v>
       </c>
-      <c r="F6" s="2"/>
+      <c r="F6" s="17" t="s">
+        <v>145</v>
+      </c>
       <c r="G6" s="2" t="s">
-        <v>144</v>
+        <v>146</v>
       </c>
       <c r="H6" s="2" t="s">
         <v>114</v>
@@ -3406,7 +3425,7 @@
       <c r="L6" s="2"/>
       <c r="M6" s="2"/>
       <c r="N6" s="2" t="s">
-        <v>145</v>
+        <v>147</v>
       </c>
       <c r="O6" s="2"/>
       <c r="P6" s="2"/>
@@ -3416,8 +3435,11 @@
       <c r="C7" s="2" t="s">
         <v>119</v>
       </c>
+      <c r="F7" s="17" t="s">
+        <v>148</v>
+      </c>
       <c r="G7" s="2" t="s">
-        <v>146</v>
+        <v>149</v>
       </c>
       <c r="K7" s="2" t="s">
         <v>55</v>
@@ -3431,13 +3453,13 @@
     </row>
     <row r="8" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="G8" s="2" t="s">
-        <v>147</v>
+        <v>150</v>
       </c>
       <c r="K8" s="2" t="s">
         <v>61</v>
       </c>
       <c r="N8" s="2" t="s">
-        <v>148</v>
+        <v>151</v>
       </c>
       <c r="O8" s="2"/>
       <c r="P8" s="19"/>
@@ -3487,7 +3509,7 @@
   <sheetData>
     <row r="1" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="7" t="s">
-        <v>149</v>
+        <v>152</v>
       </c>
       <c r="B1" s="7" t="s">
         <v>28</v>
@@ -3526,7 +3548,7 @@
     </row>
     <row r="2" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="2" t="s">
-        <v>150</v>
+        <v>153</v>
       </c>
       <c r="B2" s="2" t="s">
         <v>38</v>
@@ -3534,25 +3556,25 @@
       <c r="C2" s="2" t="s">
         <v>33</v>
       </c>
-      <c r="D2" s="16" t="s">
+      <c r="D2" s="15" t="s">
         <v>39</v>
       </c>
       <c r="E2" s="2" t="s">
         <v>129</v>
       </c>
       <c r="F2" s="2" t="s">
-        <v>151</v>
-      </c>
-      <c r="G2" s="17" t="s">
+        <v>154</v>
+      </c>
+      <c r="G2" s="16" t="s">
         <v>36</v>
       </c>
-      <c r="H2" s="17" t="s">
+      <c r="H2" s="16" t="s">
         <v>130</v>
       </c>
-      <c r="I2" s="17" t="s">
+      <c r="I2" s="16" t="s">
         <v>37</v>
       </c>
-      <c r="J2" s="17" t="s">
+      <c r="J2" s="16" t="s">
         <v>131</v>
       </c>
       <c r="K2" s="8"/>
@@ -3571,25 +3593,25 @@
       <c r="C3" s="2" t="s">
         <v>42</v>
       </c>
-      <c r="D3" s="16" t="s">
+      <c r="D3" s="15" t="s">
         <v>43</v>
       </c>
       <c r="E3" s="2" t="s">
         <v>90</v>
       </c>
       <c r="F3" s="2" t="s">
-        <v>152</v>
-      </c>
-      <c r="G3" s="17" t="s">
-        <v>153</v>
-      </c>
-      <c r="H3" s="17" t="s">
+        <v>155</v>
+      </c>
+      <c r="G3" s="16" t="s">
+        <v>156</v>
+      </c>
+      <c r="H3" s="16" t="s">
         <v>134</v>
       </c>
-      <c r="I3" s="17" t="s">
-        <v>153</v>
-      </c>
-      <c r="J3" s="17" t="s">
+      <c r="I3" s="16" t="s">
+        <v>156</v>
+      </c>
+      <c r="J3" s="16" t="s">
         <v>134</v>
       </c>
       <c r="K3" s="8"/>
@@ -3608,7 +3630,7 @@
       <c r="C4" s="2" t="s">
         <v>48</v>
       </c>
-      <c r="D4" s="16" t="s">
+      <c r="D4" s="15" t="s">
         <v>49</v>
       </c>
       <c r="E4" s="2" t="s">
@@ -3617,16 +3639,16 @@
       <c r="F4" s="2" t="s">
         <v>86</v>
       </c>
-      <c r="G4" s="17" t="s">
+      <c r="G4" s="16" t="s">
         <v>51</v>
       </c>
-      <c r="H4" s="17" t="s">
+      <c r="H4" s="16" t="s">
         <v>138</v>
       </c>
-      <c r="I4" s="17" t="s">
+      <c r="I4" s="16" t="s">
         <v>52</v>
       </c>
-      <c r="J4" s="17" t="s">
+      <c r="J4" s="16" t="s">
         <v>138</v>
       </c>
       <c r="K4" s="8"/>
@@ -3643,24 +3665,24 @@
         <v>114</v>
       </c>
       <c r="C5" s="2" t="s">
-        <v>154</v>
-      </c>
-      <c r="D5" s="16" t="s">
+        <v>157</v>
+      </c>
+      <c r="D5" s="15" t="s">
         <v>55</v>
       </c>
       <c r="E5" s="2" t="s">
-        <v>142</v>
+        <v>143</v>
       </c>
       <c r="F5" s="2" t="s">
-        <v>155</v>
-      </c>
-      <c r="G5" s="17" t="s">
+        <v>158</v>
+      </c>
+      <c r="G5" s="16" t="s">
         <v>57</v>
       </c>
       <c r="H5" s="2" t="s">
-        <v>143</v>
-      </c>
-      <c r="I5" s="17" t="s">
+        <v>144</v>
+      </c>
+      <c r="I5" s="16" t="s">
         <v>58</v>
       </c>
       <c r="J5" s="2" t="s">
@@ -3678,7 +3700,7 @@
       <c r="A6" s="23"/>
       <c r="B6" s="4"/>
       <c r="C6" s="4"/>
-      <c r="D6" s="16" t="s">
+      <c r="D6" s="15" t="s">
         <v>59</v>
       </c>
       <c r="E6" s="23"/>
@@ -3703,7 +3725,7 @@
       <c r="A7" s="23"/>
       <c r="B7" s="4"/>
       <c r="C7" s="4"/>
-      <c r="D7" s="16" t="s">
+      <c r="D7" s="15" t="s">
         <v>61</v>
       </c>
       <c r="E7" s="23"/>

</xml_diff>

<commit_message>
Removed answer key from  Admin DB
</commit_message>
<xml_diff>
--- a/OAES Database Design.xlsx
+++ b/OAES Database Design.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="299" uniqueCount="156">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="296" uniqueCount="153">
   <si>
     <t xml:space="preserve">oaes_user</t>
   </si>
@@ -329,7 +329,7 @@
     <t xml:space="preserve">examinee_batch_id FK refers EXAMINEE_BATCH</t>
   </si>
   <si>
-    <t xml:space="preserve">true_percentage</t>
+    <t xml:space="preserve">item_true_false_code UNIQUE NOTNULL</t>
   </si>
   <si>
     <t xml:space="preserve">exam_drive_code UNIQUE NOTNULL</t>
@@ -353,10 +353,7 @@
     <t xml:space="preserve">itemtype_code UNIQUE NOTNULL</t>
   </si>
   <si>
-    <t xml:space="preserve">mcq_option_percentage</t>
-  </si>
-  <si>
-    <t xml:space="preserve">false_percentage</t>
+    <t xml:space="preserve">item_mcq_options_code UNIQUE NOTNULL</t>
   </si>
   <si>
     <t xml:space="preserve">course_master_id FK refers COURSE_MASTER</t>
@@ -369,12 +366,6 @@
   </si>
   <si>
     <t xml:space="preserve">qp_code UNIQUE NOTNULL</t>
-  </si>
-  <si>
-    <t xml:space="preserve">item_mcq_options_code UNIQUE NOTNULL</t>
-  </si>
-  <si>
-    <t xml:space="preserve">item_true_false_code UNIQUE NOTNULL</t>
   </si>
   <si>
     <t xml:space="preserve">examinee_email</t>
@@ -676,7 +667,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="28">
+  <cellXfs count="27">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -719,10 +710,6 @@
     </xf>
     <xf numFmtId="164" fontId="6" fillId="4" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="5" fillId="4" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
@@ -1501,8 +1488,8 @@
   </sheetPr>
   <dimension ref="A1:AC14"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="D1" colorId="64" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="E17" activeCellId="0" sqref="E17"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="K1" colorId="64" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="L18" activeCellId="0" sqref="L18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -1518,7 +1505,7 @@
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="0" width="35.23"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="0" width="76.92"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="11" min="11" style="0" width="45.84"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="12" min="12" style="0" width="35"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="12" min="12" style="0" width="41.42"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="13" min="13" style="0" width="39.16"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1022" min="14" style="0" width="14.43"/>
     <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1025" min="1023" style="0" width="11.52"/>
@@ -1787,9 +1774,7 @@
       <c r="L5" s="2" t="s">
         <v>109</v>
       </c>
-      <c r="M5" s="2" t="s">
-        <v>110</v>
-      </c>
+      <c r="M5" s="4"/>
       <c r="N5" s="8"/>
       <c r="O5" s="8"/>
       <c r="P5" s="8"/>
@@ -1810,18 +1795,18 @@
     <row r="6" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="4"/>
       <c r="B6" s="2" t="s">
+        <v>110</v>
+      </c>
+      <c r="C6" s="2" t="s">
         <v>111</v>
-      </c>
-      <c r="C6" s="2" t="s">
-        <v>112</v>
       </c>
       <c r="D6" s="4"/>
       <c r="E6" s="2" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="F6" s="10"/>
       <c r="G6" s="2" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="H6" s="4"/>
       <c r="I6" s="4"/>
@@ -1829,12 +1814,8 @@
         <v>55</v>
       </c>
       <c r="K6" s="10"/>
-      <c r="L6" s="2" t="s">
-        <v>115</v>
-      </c>
-      <c r="M6" s="2" t="s">
-        <v>116</v>
-      </c>
+      <c r="L6" s="4"/>
+      <c r="M6" s="4"/>
       <c r="N6" s="8"/>
       <c r="O6" s="8"/>
       <c r="P6" s="8"/>
@@ -1856,11 +1837,11 @@
       <c r="A7" s="4"/>
       <c r="B7" s="4"/>
       <c r="C7" s="2" t="s">
-        <v>117</v>
+        <v>114</v>
       </c>
       <c r="D7" s="4"/>
       <c r="E7" s="2" t="s">
-        <v>118</v>
+        <v>115</v>
       </c>
       <c r="F7" s="4"/>
       <c r="G7" s="4"/>
@@ -1893,18 +1874,18 @@
       <c r="A8" s="4"/>
       <c r="B8" s="4"/>
       <c r="C8" s="8" t="s">
-        <v>119</v>
+        <v>116</v>
       </c>
       <c r="D8" s="4"/>
-      <c r="E8" s="11" t="s">
-        <v>120</v>
+      <c r="E8" s="2" t="s">
+        <v>117</v>
       </c>
       <c r="F8" s="4"/>
       <c r="G8" s="4"/>
       <c r="H8" s="4"/>
       <c r="I8" s="4"/>
       <c r="J8" s="2" t="s">
-        <v>121</v>
+        <v>118</v>
       </c>
       <c r="K8" s="4"/>
       <c r="L8" s="4"/>
@@ -2052,7 +2033,7 @@
     </row>
     <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="4"/>
-      <c r="B13" s="12"/>
+      <c r="B13" s="11"/>
       <c r="C13" s="4"/>
       <c r="D13" s="4"/>
       <c r="E13" s="4"/>
@@ -3142,7 +3123,7 @@
         <v>71</v>
       </c>
       <c r="G1" s="7" t="s">
-        <v>122</v>
+        <v>119</v>
       </c>
       <c r="H1" s="7" t="s">
         <v>28</v>
@@ -3153,7 +3134,7 @@
       <c r="J1" s="7" t="s">
         <v>23</v>
       </c>
-      <c r="K1" s="13" t="s">
+      <c r="K1" s="12" t="s">
         <v>29</v>
       </c>
       <c r="L1" s="7" t="s">
@@ -3162,17 +3143,17 @@
       <c r="M1" s="7" t="s">
         <v>27</v>
       </c>
-      <c r="N1" s="14" t="s">
+      <c r="N1" s="13" t="s">
+        <v>120</v>
+      </c>
+      <c r="O1" s="1" t="s">
+        <v>121</v>
+      </c>
+      <c r="P1" s="14" t="s">
+        <v>122</v>
+      </c>
+      <c r="Q1" s="14" t="s">
         <v>123</v>
-      </c>
-      <c r="O1" s="1" t="s">
-        <v>124</v>
-      </c>
-      <c r="P1" s="15" t="s">
-        <v>125</v>
-      </c>
-      <c r="Q1" s="15" t="s">
-        <v>126</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3195,7 +3176,7 @@
         <v>79</v>
       </c>
       <c r="G2" s="2" t="s">
-        <v>127</v>
+        <v>124</v>
       </c>
       <c r="H2" s="2" t="s">
         <v>38</v>
@@ -3206,7 +3187,7 @@
       <c r="J2" s="2" t="s">
         <v>33</v>
       </c>
-      <c r="K2" s="16" t="s">
+      <c r="K2" s="15" t="s">
         <v>39</v>
       </c>
       <c r="L2" s="2" t="s">
@@ -3215,17 +3196,17 @@
       <c r="M2" s="2" t="s">
         <v>37</v>
       </c>
-      <c r="N2" s="16" t="s">
+      <c r="N2" s="15" t="s">
+        <v>125</v>
+      </c>
+      <c r="O2" s="2" t="s">
+        <v>126</v>
+      </c>
+      <c r="P2" s="16" t="s">
+        <v>127</v>
+      </c>
+      <c r="Q2" s="16" t="s">
         <v>128</v>
-      </c>
-      <c r="O2" s="2" t="s">
-        <v>129</v>
-      </c>
-      <c r="P2" s="17" t="s">
-        <v>130</v>
-      </c>
-      <c r="Q2" s="17" t="s">
-        <v>131</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3248,7 +3229,7 @@
         <v>87</v>
       </c>
       <c r="G3" s="2" t="s">
-        <v>132</v>
+        <v>129</v>
       </c>
       <c r="H3" s="2" t="s">
         <v>87</v>
@@ -3259,8 +3240,8 @@
       <c r="J3" s="2" t="s">
         <v>89</v>
       </c>
-      <c r="K3" s="16" t="s">
-        <v>121</v>
+      <c r="K3" s="15" t="s">
+        <v>118</v>
       </c>
       <c r="L3" s="2" t="s">
         <v>90</v>
@@ -3268,17 +3249,17 @@
       <c r="M3" s="2" t="s">
         <v>90</v>
       </c>
-      <c r="N3" s="16" t="s">
-        <v>133</v>
+      <c r="N3" s="15" t="s">
+        <v>130</v>
       </c>
       <c r="O3" s="2" t="s">
         <v>90</v>
       </c>
-      <c r="P3" s="17" t="s">
-        <v>134</v>
-      </c>
-      <c r="Q3" s="17" t="s">
-        <v>134</v>
+      <c r="P3" s="16" t="s">
+        <v>131</v>
+      </c>
+      <c r="Q3" s="16" t="s">
+        <v>131</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3301,7 +3282,7 @@
         <v>96</v>
       </c>
       <c r="G4" s="2" t="s">
-        <v>135</v>
+        <v>132</v>
       </c>
       <c r="H4" s="2" t="s">
         <v>97</v>
@@ -3319,19 +3300,19 @@
         <v>51</v>
       </c>
       <c r="M4" s="2" t="s">
-        <v>116</v>
+        <v>101</v>
       </c>
       <c r="N4" s="2" t="s">
+        <v>133</v>
+      </c>
+      <c r="O4" s="2" t="s">
+        <v>134</v>
+      </c>
+      <c r="P4" s="16" t="s">
+        <v>135</v>
+      </c>
+      <c r="Q4" s="16" t="s">
         <v>136</v>
-      </c>
-      <c r="O4" s="2" t="s">
-        <v>137</v>
-      </c>
-      <c r="P4" s="17" t="s">
-        <v>138</v>
-      </c>
-      <c r="Q4" s="17" t="s">
-        <v>139</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3350,7 +3331,7 @@
       </c>
       <c r="F5" s="2"/>
       <c r="G5" s="3" t="s">
-        <v>140</v>
+        <v>137</v>
       </c>
       <c r="H5" s="2" t="s">
         <v>106</v>
@@ -3365,38 +3346,38 @@
         <v>49</v>
       </c>
       <c r="L5" s="2" t="s">
-        <v>115</v>
+        <v>109</v>
       </c>
       <c r="M5" s="2"/>
       <c r="N5" s="2" t="s">
-        <v>141</v>
+        <v>138</v>
       </c>
       <c r="O5" s="2" t="s">
-        <v>142</v>
+        <v>139</v>
       </c>
       <c r="P5" s="2" t="s">
-        <v>143</v>
-      </c>
-      <c r="Q5" s="18"/>
+        <v>140</v>
+      </c>
+      <c r="Q5" s="17"/>
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="2"/>
       <c r="B6" s="2" t="s">
+        <v>110</v>
+      </c>
+      <c r="C6" s="2" t="s">
         <v>111</v>
-      </c>
-      <c r="C6" s="2" t="s">
-        <v>112</v>
       </c>
       <c r="D6" s="2"/>
       <c r="E6" s="2" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="F6" s="2"/>
       <c r="G6" s="2" t="s">
-        <v>144</v>
+        <v>141</v>
       </c>
       <c r="H6" s="2" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="I6" s="2"/>
       <c r="J6" s="2"/>
@@ -3406,7 +3387,7 @@
       <c r="L6" s="2"/>
       <c r="M6" s="2"/>
       <c r="N6" s="2" t="s">
-        <v>145</v>
+        <v>142</v>
       </c>
       <c r="O6" s="2"/>
       <c r="P6" s="2"/>
@@ -3414,10 +3395,10 @@
     </row>
     <row r="7" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C7" s="2" t="s">
-        <v>119</v>
+        <v>116</v>
       </c>
       <c r="G7" s="2" t="s">
-        <v>146</v>
+        <v>143</v>
       </c>
       <c r="K7" s="2" t="s">
         <v>55</v>
@@ -3426,22 +3407,22 @@
         <v>100</v>
       </c>
       <c r="O7" s="2"/>
-      <c r="P7" s="19"/>
-      <c r="Q7" s="19"/>
+      <c r="P7" s="18"/>
+      <c r="Q7" s="18"/>
     </row>
     <row r="8" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="G8" s="2" t="s">
-        <v>147</v>
+        <v>144</v>
       </c>
       <c r="K8" s="2" t="s">
         <v>61</v>
       </c>
       <c r="N8" s="2" t="s">
-        <v>148</v>
+        <v>145</v>
       </c>
       <c r="O8" s="2"/>
-      <c r="P8" s="19"/>
-      <c r="Q8" s="19"/>
+      <c r="P8" s="18"/>
+      <c r="Q8" s="18"/>
     </row>
   </sheetData>
   <conditionalFormatting sqref="G2:G7 K8 N8">
@@ -3487,7 +3468,7 @@
   <sheetData>
     <row r="1" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="7" t="s">
-        <v>149</v>
+        <v>146</v>
       </c>
       <c r="B1" s="7" t="s">
         <v>28</v>
@@ -3495,26 +3476,26 @@
       <c r="C1" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="D1" s="20" t="s">
+      <c r="D1" s="19" t="s">
         <v>29</v>
       </c>
       <c r="E1" s="7" t="s">
-        <v>124</v>
+        <v>121</v>
       </c>
       <c r="F1" s="7" t="s">
         <v>73</v>
       </c>
-      <c r="G1" s="21" t="s">
+      <c r="G1" s="20" t="s">
         <v>26</v>
       </c>
-      <c r="H1" s="21" t="s">
-        <v>125</v>
-      </c>
-      <c r="I1" s="21" t="s">
+      <c r="H1" s="20" t="s">
+        <v>122</v>
+      </c>
+      <c r="I1" s="20" t="s">
         <v>27</v>
       </c>
-      <c r="J1" s="21" t="s">
-        <v>126</v>
+      <c r="J1" s="20" t="s">
+        <v>123</v>
       </c>
       <c r="K1" s="8"/>
       <c r="L1" s="8"/>
@@ -3526,7 +3507,7 @@
     </row>
     <row r="2" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="2" t="s">
-        <v>150</v>
+        <v>147</v>
       </c>
       <c r="B2" s="2" t="s">
         <v>38</v>
@@ -3534,26 +3515,26 @@
       <c r="C2" s="2" t="s">
         <v>33</v>
       </c>
-      <c r="D2" s="16" t="s">
+      <c r="D2" s="15" t="s">
         <v>39</v>
       </c>
       <c r="E2" s="2" t="s">
-        <v>129</v>
+        <v>126</v>
       </c>
       <c r="F2" s="2" t="s">
-        <v>151</v>
-      </c>
-      <c r="G2" s="17" t="s">
+        <v>148</v>
+      </c>
+      <c r="G2" s="16" t="s">
         <v>36</v>
       </c>
-      <c r="H2" s="17" t="s">
-        <v>130</v>
-      </c>
-      <c r="I2" s="17" t="s">
+      <c r="H2" s="16" t="s">
+        <v>127</v>
+      </c>
+      <c r="I2" s="16" t="s">
         <v>37</v>
       </c>
-      <c r="J2" s="17" t="s">
-        <v>131</v>
+      <c r="J2" s="16" t="s">
+        <v>128</v>
       </c>
       <c r="K2" s="8"/>
       <c r="L2" s="8"/>
@@ -3571,26 +3552,26 @@
       <c r="C3" s="2" t="s">
         <v>42</v>
       </c>
-      <c r="D3" s="16" t="s">
+      <c r="D3" s="15" t="s">
         <v>43</v>
       </c>
       <c r="E3" s="2" t="s">
         <v>90</v>
       </c>
       <c r="F3" s="2" t="s">
-        <v>152</v>
-      </c>
-      <c r="G3" s="17" t="s">
-        <v>153</v>
-      </c>
-      <c r="H3" s="17" t="s">
-        <v>134</v>
-      </c>
-      <c r="I3" s="17" t="s">
-        <v>153</v>
-      </c>
-      <c r="J3" s="17" t="s">
-        <v>134</v>
+        <v>149</v>
+      </c>
+      <c r="G3" s="16" t="s">
+        <v>150</v>
+      </c>
+      <c r="H3" s="16" t="s">
+        <v>131</v>
+      </c>
+      <c r="I3" s="16" t="s">
+        <v>150</v>
+      </c>
+      <c r="J3" s="16" t="s">
+        <v>131</v>
       </c>
       <c r="K3" s="8"/>
       <c r="L3" s="8"/>
@@ -3608,7 +3589,7 @@
       <c r="C4" s="2" t="s">
         <v>48</v>
       </c>
-      <c r="D4" s="16" t="s">
+      <c r="D4" s="15" t="s">
         <v>49</v>
       </c>
       <c r="E4" s="2" t="s">
@@ -3617,17 +3598,17 @@
       <c r="F4" s="2" t="s">
         <v>86</v>
       </c>
-      <c r="G4" s="17" t="s">
+      <c r="G4" s="16" t="s">
         <v>51</v>
       </c>
-      <c r="H4" s="17" t="s">
-        <v>138</v>
-      </c>
-      <c r="I4" s="17" t="s">
+      <c r="H4" s="16" t="s">
+        <v>135</v>
+      </c>
+      <c r="I4" s="16" t="s">
         <v>52</v>
       </c>
-      <c r="J4" s="17" t="s">
-        <v>138</v>
+      <c r="J4" s="16" t="s">
+        <v>135</v>
       </c>
       <c r="K4" s="8"/>
       <c r="L4" s="8"/>
@@ -3638,33 +3619,33 @@
       <c r="Q4" s="8"/>
     </row>
     <row r="5" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="22"/>
+      <c r="A5" s="21"/>
       <c r="B5" s="2" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="C5" s="2" t="s">
-        <v>154</v>
-      </c>
-      <c r="D5" s="16" t="s">
+        <v>151</v>
+      </c>
+      <c r="D5" s="15" t="s">
         <v>55</v>
       </c>
       <c r="E5" s="2" t="s">
-        <v>142</v>
+        <v>139</v>
       </c>
       <c r="F5" s="2" t="s">
-        <v>155</v>
-      </c>
-      <c r="G5" s="17" t="s">
+        <v>152</v>
+      </c>
+      <c r="G5" s="16" t="s">
         <v>57</v>
       </c>
       <c r="H5" s="2" t="s">
-        <v>143</v>
-      </c>
-      <c r="I5" s="17" t="s">
+        <v>140</v>
+      </c>
+      <c r="I5" s="16" t="s">
         <v>58</v>
       </c>
       <c r="J5" s="2" t="s">
-        <v>139</v>
+        <v>136</v>
       </c>
       <c r="K5" s="8"/>
       <c r="L5" s="8"/>
@@ -3675,22 +3656,22 @@
       <c r="Q5" s="8"/>
     </row>
     <row r="6" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A6" s="23"/>
+      <c r="A6" s="22"/>
       <c r="B6" s="4"/>
       <c r="C6" s="4"/>
-      <c r="D6" s="16" t="s">
+      <c r="D6" s="15" t="s">
         <v>59</v>
       </c>
-      <c r="E6" s="23"/>
-      <c r="F6" s="23"/>
+      <c r="E6" s="22"/>
+      <c r="F6" s="22"/>
       <c r="G6" s="2" t="s">
-        <v>115</v>
-      </c>
-      <c r="H6" s="24"/>
+        <v>109</v>
+      </c>
+      <c r="H6" s="23"/>
       <c r="I6" s="2" t="s">
-        <v>116</v>
-      </c>
-      <c r="J6" s="25"/>
+        <v>101</v>
+      </c>
+      <c r="J6" s="24"/>
       <c r="K6" s="8"/>
       <c r="L6" s="8"/>
       <c r="M6" s="8"/>
@@ -3700,18 +3681,18 @@
       <c r="Q6" s="8"/>
     </row>
     <row r="7" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A7" s="23"/>
+      <c r="A7" s="22"/>
       <c r="B7" s="4"/>
       <c r="C7" s="4"/>
-      <c r="D7" s="16" t="s">
+      <c r="D7" s="15" t="s">
         <v>61</v>
       </c>
-      <c r="E7" s="23"/>
-      <c r="F7" s="23"/>
-      <c r="G7" s="25"/>
-      <c r="H7" s="25"/>
-      <c r="I7" s="25"/>
-      <c r="J7" s="25"/>
+      <c r="E7" s="22"/>
+      <c r="F7" s="22"/>
+      <c r="G7" s="24"/>
+      <c r="H7" s="24"/>
+      <c r="I7" s="24"/>
+      <c r="J7" s="24"/>
       <c r="K7" s="8"/>
       <c r="L7" s="8"/>
       <c r="M7" s="8"/>
@@ -3721,7 +3702,7 @@
       <c r="Q7" s="8"/>
     </row>
     <row r="8" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A8" s="23"/>
+      <c r="A8" s="22"/>
       <c r="B8" s="4"/>
       <c r="C8" s="4"/>
       <c r="D8" s="2" t="s">
@@ -3729,10 +3710,10 @@
       </c>
       <c r="E8" s="4"/>
       <c r="F8" s="4"/>
-      <c r="G8" s="25"/>
-      <c r="H8" s="25"/>
-      <c r="I8" s="25"/>
-      <c r="J8" s="25"/>
+      <c r="G8" s="24"/>
+      <c r="H8" s="24"/>
+      <c r="I8" s="24"/>
+      <c r="J8" s="24"/>
       <c r="K8" s="8"/>
       <c r="L8" s="8"/>
       <c r="M8" s="8"/>
@@ -3745,13 +3726,13 @@
       <c r="A9" s="4"/>
       <c r="B9" s="4"/>
       <c r="C9" s="4"/>
-      <c r="D9" s="26"/>
+      <c r="D9" s="25"/>
       <c r="E9" s="4"/>
       <c r="F9" s="4"/>
-      <c r="G9" s="25"/>
-      <c r="H9" s="25"/>
-      <c r="I9" s="25"/>
-      <c r="J9" s="25"/>
+      <c r="G9" s="24"/>
+      <c r="H9" s="24"/>
+      <c r="I9" s="24"/>
+      <c r="J9" s="24"/>
       <c r="K9" s="8"/>
       <c r="L9" s="8"/>
       <c r="M9" s="8"/>
@@ -3764,13 +3745,13 @@
       <c r="A10" s="4"/>
       <c r="B10" s="4"/>
       <c r="C10" s="4"/>
-      <c r="D10" s="26"/>
+      <c r="D10" s="25"/>
       <c r="E10" s="4"/>
       <c r="F10" s="4"/>
-      <c r="G10" s="25"/>
-      <c r="H10" s="25"/>
-      <c r="I10" s="25"/>
-      <c r="J10" s="25"/>
+      <c r="G10" s="24"/>
+      <c r="H10" s="24"/>
+      <c r="I10" s="24"/>
+      <c r="J10" s="24"/>
       <c r="K10" s="8"/>
       <c r="L10" s="8"/>
       <c r="M10" s="8"/>
@@ -3783,13 +3764,13 @@
       <c r="A11" s="4"/>
       <c r="B11" s="4"/>
       <c r="C11" s="4"/>
-      <c r="D11" s="26"/>
+      <c r="D11" s="25"/>
       <c r="E11" s="4"/>
       <c r="F11" s="4"/>
-      <c r="G11" s="25"/>
-      <c r="H11" s="25"/>
-      <c r="I11" s="25"/>
-      <c r="J11" s="25"/>
+      <c r="G11" s="24"/>
+      <c r="H11" s="24"/>
+      <c r="I11" s="24"/>
+      <c r="J11" s="24"/>
       <c r="K11" s="8"/>
       <c r="L11" s="8"/>
       <c r="M11" s="8"/>
@@ -3802,13 +3783,13 @@
       <c r="A12" s="4"/>
       <c r="B12" s="4"/>
       <c r="C12" s="4"/>
-      <c r="D12" s="27"/>
+      <c r="D12" s="26"/>
       <c r="E12" s="4"/>
       <c r="F12" s="4"/>
-      <c r="G12" s="25"/>
-      <c r="H12" s="25"/>
-      <c r="I12" s="25"/>
-      <c r="J12" s="25"/>
+      <c r="G12" s="24"/>
+      <c r="H12" s="24"/>
+      <c r="I12" s="24"/>
+      <c r="J12" s="24"/>
       <c r="K12" s="8"/>
       <c r="L12" s="8"/>
       <c r="M12" s="8"/>
@@ -3821,13 +3802,13 @@
       <c r="A13" s="4"/>
       <c r="B13" s="4"/>
       <c r="C13" s="4"/>
-      <c r="D13" s="27"/>
+      <c r="D13" s="26"/>
       <c r="E13" s="4"/>
       <c r="F13" s="4"/>
-      <c r="G13" s="25"/>
-      <c r="H13" s="25"/>
-      <c r="I13" s="25"/>
-      <c r="J13" s="25"/>
+      <c r="G13" s="24"/>
+      <c r="H13" s="24"/>
+      <c r="I13" s="24"/>
+      <c r="J13" s="24"/>
       <c r="K13" s="8"/>
       <c r="L13" s="8"/>
       <c r="M13" s="8"/>

</xml_diff>

<commit_message>
DB Update - Link Batch and Examdrive
</commit_message>
<xml_diff>
--- a/OAES Database Design.xlsx
+++ b/OAES Database Design.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="302" uniqueCount="159">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="301" uniqueCount="162">
   <si>
     <t xml:space="preserve">oaes_user</t>
   </si>
@@ -422,6 +422,9 @@
     <t xml:space="preserve">response_true_false_id PK</t>
   </si>
   <si>
+    <t xml:space="preserve">center_id FK refers CENTER</t>
+  </si>
+  <si>
     <t xml:space="preserve">invigilator_name</t>
   </si>
   <si>
@@ -431,6 +434,9 @@
     <t xml:space="preserve">response_id FK referes RESPONSE</t>
   </si>
   <si>
+    <t xml:space="preserve">status (NOT STARTED, IN_PROGRESS, COMPLETED)</t>
+  </si>
+  <si>
     <t xml:space="preserve">invigilator_email</t>
   </si>
   <si>
@@ -443,64 +449,67 @@
     <t xml:space="preserve">response_text</t>
   </si>
   <si>
+    <t xml:space="preserve">examinee_batch_start_time</t>
+  </si>
+  <si>
+    <t xml:space="preserve">invigilator_password</t>
+  </si>
+  <si>
+    <t xml:space="preserve">attempt_start_time</t>
+  </si>
+  <si>
+    <t xml:space="preserve">examinee_batch_end_time</t>
+  </si>
+  <si>
+    <t xml:space="preserve">batch_id FK refers BATCH_COURSE</t>
+  </si>
+  <si>
+    <t xml:space="preserve">attempt_end_time</t>
+  </si>
+  <si>
+    <t xml:space="preserve">examdrive_id FK refers EXAMDRIVE</t>
+  </si>
+  <si>
+    <t xml:space="preserve">examinee_batch_status(NOT_Started, IN_Progress,Completed)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">user_status(Active, NOT_Active)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">qp_id FK refers QUESTIONPAPER</t>
+  </si>
+  <si>
+    <t xml:space="preserve">invigilator_code UNIQUE NOTNULL</t>
+  </si>
+  <si>
+    <t xml:space="preserve">drive_center_examinee</t>
+  </si>
+  <si>
+    <t xml:space="preserve">drive_center_examinee_id PK</t>
+  </si>
+  <si>
+    <t xml:space="preserve">examinee_item_id PK</t>
+  </si>
+  <si>
+    <t xml:space="preserve">drive_center_examiniee_id PK FK refers DRIVE_CENTER_EXAMINEE</t>
+  </si>
+  <si>
+    <t xml:space="preserve">qp_item_id FK referes QP_ITEM</t>
+  </si>
+  <si>
+    <t xml:space="preserve">item_type_code UNIQUE NOTNULL</t>
+  </si>
+  <si>
+    <t xml:space="preserve">response_code UNIQUE NOTNULL</t>
+  </si>
+  <si>
+    <t xml:space="preserve">qp_item FK refers QP_ITEM</t>
+  </si>
+  <si>
+    <t xml:space="preserve">response_mcq_code UNIQUE NOTNULL</t>
+  </si>
+  <si>
     <t xml:space="preserve">response_true_false_code UNIQUE NOTNULL</t>
-  </si>
-  <si>
-    <t xml:space="preserve">examinee_batch_start_time</t>
-  </si>
-  <si>
-    <t xml:space="preserve">invigilator_password</t>
-  </si>
-  <si>
-    <t xml:space="preserve">attempt_start_time</t>
-  </si>
-  <si>
-    <t xml:space="preserve">response_code UNIQUE NOTNULL</t>
-  </si>
-  <si>
-    <t xml:space="preserve">response_mcq_code UNIQUE NOTNULL</t>
-  </si>
-  <si>
-    <t xml:space="preserve">examinee_batch_end_time</t>
-  </si>
-  <si>
-    <t xml:space="preserve">batch_id FK refers BATCH_COURSE</t>
-  </si>
-  <si>
-    <t xml:space="preserve">attempt_end_time</t>
-  </si>
-  <si>
-    <t xml:space="preserve">examinee_batch_status(NOT_Started, IN_Progress,Completed)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">user_status(Active, NOT_Active)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">invigilator_code UNIQUE NOTNULL</t>
-  </si>
-  <si>
-    <t xml:space="preserve">attempt_code UNIQUE NOTNULL</t>
-  </si>
-  <si>
-    <t xml:space="preserve">drive_center_examinee</t>
-  </si>
-  <si>
-    <t xml:space="preserve">drive_center_examinee_id PK</t>
-  </si>
-  <si>
-    <t xml:space="preserve">examinee_item_id PK</t>
-  </si>
-  <si>
-    <t xml:space="preserve">drive_center_examiniee_id PK FK refers DRIVE_CENTER_EXAMINEE</t>
-  </si>
-  <si>
-    <t xml:space="preserve">qp_item_id FK referes QP_ITEM</t>
-  </si>
-  <si>
-    <t xml:space="preserve">item_type_code UNIQUE NOTNULL</t>
-  </si>
-  <si>
-    <t xml:space="preserve">qp_item FK refers QP_ITEM</t>
   </si>
 </sst>
 </file>
@@ -571,7 +580,7 @@
       <charset val="1"/>
     </font>
     <font>
-      <sz val="10"/>
+      <sz val="11"/>
       <color rgb="FF000000"/>
       <name val="Calibri"/>
       <family val="0"/>
@@ -691,7 +700,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="28">
+  <cellXfs count="29">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -766,6 +775,10 @@
     </xf>
     <xf numFmtId="164" fontId="10" fillId="0" borderId="4" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="8" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="6" fillId="0" borderId="4" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
@@ -892,7 +905,7 @@
   </sheetPr>
   <dimension ref="A1:E13"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
@@ -1062,7 +1075,7 @@
   </sheetPr>
   <dimension ref="A1:Z1048576"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
@@ -1516,7 +1529,7 @@
   </sheetPr>
   <dimension ref="A1:AC998"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="D1" colorId="64" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="D1" colorId="64" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="E17" activeCellId="0" sqref="E17"/>
     </sheetView>
   </sheetViews>
@@ -3104,8 +3117,8 @@
   </sheetPr>
   <dimension ref="A1:Q8"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="J1" colorId="64" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="F10" activeCellId="0" sqref="F10"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="B12" activeCellId="0" sqref="B12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -3114,7 +3127,7 @@
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="39.09"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="26.82"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="24.45"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="23.91"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="32"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="48.01"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="0" width="27.64"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="0" width="21.82"/>
@@ -3257,13 +3270,13 @@
         <v>84</v>
       </c>
       <c r="E3" s="2" t="s">
-        <v>85</v>
+        <v>132</v>
       </c>
       <c r="F3" s="2" t="s">
         <v>87</v>
       </c>
       <c r="G3" s="2" t="s">
-        <v>132</v>
+        <v>133</v>
       </c>
       <c r="H3" s="2" t="s">
         <v>87</v>
@@ -3284,16 +3297,16 @@
         <v>90</v>
       </c>
       <c r="N3" s="15" t="s">
-        <v>133</v>
+        <v>134</v>
       </c>
       <c r="O3" s="2" t="s">
         <v>90</v>
       </c>
       <c r="P3" s="16" t="s">
-        <v>134</v>
+        <v>135</v>
       </c>
       <c r="Q3" s="16" t="s">
-        <v>134</v>
+        <v>135</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3301,7 +3314,7 @@
         <v>91</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>92</v>
+        <v>136</v>
       </c>
       <c r="C4" s="2" t="s">
         <v>93</v>
@@ -3316,7 +3329,7 @@
         <v>96</v>
       </c>
       <c r="G4" s="2" t="s">
-        <v>135</v>
+        <v>137</v>
       </c>
       <c r="H4" s="2" t="s">
         <v>97</v>
@@ -3337,17 +3350,15 @@
         <v>116</v>
       </c>
       <c r="N4" s="2" t="s">
-        <v>136</v>
+        <v>138</v>
       </c>
       <c r="O4" s="2" t="s">
-        <v>137</v>
+        <v>139</v>
       </c>
       <c r="P4" s="16" t="s">
-        <v>138</v>
-      </c>
-      <c r="Q4" s="16" t="s">
-        <v>139</v>
-      </c>
+        <v>140</v>
+      </c>
+      <c r="Q4" s="16"/>
     </row>
     <row r="5" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="2"/>
@@ -3363,11 +3374,11 @@
       <c r="E5" s="2" t="s">
         <v>105</v>
       </c>
-      <c r="F5" s="17" t="s">
-        <v>140</v>
+      <c r="F5" s="2" t="s">
+        <v>141</v>
       </c>
       <c r="G5" s="3" t="s">
-        <v>141</v>
+        <v>142</v>
       </c>
       <c r="H5" s="2" t="s">
         <v>106</v>
@@ -3386,17 +3397,15 @@
       </c>
       <c r="M5" s="2"/>
       <c r="N5" s="2" t="s">
-        <v>142</v>
-      </c>
-      <c r="O5" s="2" t="s">
         <v>143</v>
       </c>
-      <c r="P5" s="2" t="s">
-        <v>144</v>
-      </c>
+      <c r="O5" s="17" t="s">
+        <v>140</v>
+      </c>
+      <c r="P5" s="2"/>
       <c r="Q5" s="18"/>
     </row>
-    <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="6" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="2"/>
       <c r="B6" s="2" t="s">
         <v>111</v>
@@ -3408,11 +3417,11 @@
       <c r="E6" s="2" t="s">
         <v>113</v>
       </c>
-      <c r="F6" s="17" t="s">
+      <c r="F6" s="2" t="s">
+        <v>144</v>
+      </c>
+      <c r="G6" s="2" t="s">
         <v>145</v>
-      </c>
-      <c r="G6" s="2" t="s">
-        <v>146</v>
       </c>
       <c r="H6" s="2" t="s">
         <v>114</v>
@@ -3425,9 +3434,9 @@
       <c r="L6" s="2"/>
       <c r="M6" s="2"/>
       <c r="N6" s="2" t="s">
-        <v>147</v>
-      </c>
-      <c r="O6" s="2"/>
+        <v>146</v>
+      </c>
+      <c r="O6" s="19"/>
       <c r="P6" s="2"/>
       <c r="Q6" s="2"/>
     </row>
@@ -3435,7 +3444,10 @@
       <c r="C7" s="2" t="s">
         <v>119</v>
       </c>
-      <c r="F7" s="17" t="s">
+      <c r="E7" s="0" t="s">
+        <v>147</v>
+      </c>
+      <c r="F7" s="2" t="s">
         <v>148</v>
       </c>
       <c r="G7" s="2" t="s">
@@ -3448,22 +3460,23 @@
         <v>100</v>
       </c>
       <c r="O7" s="2"/>
-      <c r="P7" s="19"/>
-      <c r="Q7" s="19"/>
+      <c r="P7" s="20"/>
+      <c r="Q7" s="20"/>
     </row>
     <row r="8" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="E8" s="0" t="s">
+        <v>150</v>
+      </c>
       <c r="G8" s="2" t="s">
-        <v>150</v>
+        <v>151</v>
       </c>
       <c r="K8" s="2" t="s">
         <v>61</v>
       </c>
-      <c r="N8" s="2" t="s">
-        <v>151</v>
-      </c>
+      <c r="N8" s="2"/>
       <c r="O8" s="2"/>
-      <c r="P8" s="19"/>
-      <c r="Q8" s="19"/>
+      <c r="P8" s="20"/>
+      <c r="Q8" s="20"/>
     </row>
   </sheetData>
   <conditionalFormatting sqref="G2:G7 K8 N8">
@@ -3488,7 +3501,7 @@
   </sheetPr>
   <dimension ref="A1:Q1048576"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
@@ -3517,7 +3530,7 @@
       <c r="C1" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="D1" s="20" t="s">
+      <c r="D1" s="21" t="s">
         <v>29</v>
       </c>
       <c r="E1" s="7" t="s">
@@ -3526,16 +3539,16 @@
       <c r="F1" s="7" t="s">
         <v>73</v>
       </c>
-      <c r="G1" s="21" t="s">
+      <c r="G1" s="22" t="s">
         <v>26</v>
       </c>
-      <c r="H1" s="21" t="s">
+      <c r="H1" s="22" t="s">
         <v>125</v>
       </c>
-      <c r="I1" s="21" t="s">
+      <c r="I1" s="22" t="s">
         <v>27</v>
       </c>
-      <c r="J1" s="21" t="s">
+      <c r="J1" s="22" t="s">
         <v>126</v>
       </c>
       <c r="K1" s="8"/>
@@ -3606,13 +3619,13 @@
         <v>156</v>
       </c>
       <c r="H3" s="16" t="s">
-        <v>134</v>
+        <v>135</v>
       </c>
       <c r="I3" s="16" t="s">
         <v>156</v>
       </c>
       <c r="J3" s="16" t="s">
-        <v>134</v>
+        <v>135</v>
       </c>
       <c r="K3" s="8"/>
       <c r="L3" s="8"/>
@@ -3643,13 +3656,13 @@
         <v>51</v>
       </c>
       <c r="H4" s="16" t="s">
-        <v>138</v>
+        <v>140</v>
       </c>
       <c r="I4" s="16" t="s">
         <v>52</v>
       </c>
       <c r="J4" s="16" t="s">
-        <v>138</v>
+        <v>140</v>
       </c>
       <c r="K4" s="8"/>
       <c r="L4" s="8"/>
@@ -3660,7 +3673,7 @@
       <c r="Q4" s="8"/>
     </row>
     <row r="5" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="22"/>
+      <c r="A5" s="23"/>
       <c r="B5" s="2" t="s">
         <v>114</v>
       </c>
@@ -3671,22 +3684,22 @@
         <v>55</v>
       </c>
       <c r="E5" s="2" t="s">
-        <v>143</v>
+        <v>158</v>
       </c>
       <c r="F5" s="2" t="s">
-        <v>158</v>
+        <v>159</v>
       </c>
       <c r="G5" s="16" t="s">
         <v>57</v>
       </c>
       <c r="H5" s="2" t="s">
-        <v>144</v>
+        <v>160</v>
       </c>
       <c r="I5" s="16" t="s">
         <v>58</v>
       </c>
       <c r="J5" s="2" t="s">
-        <v>139</v>
+        <v>161</v>
       </c>
       <c r="K5" s="8"/>
       <c r="L5" s="8"/>
@@ -3697,22 +3710,22 @@
       <c r="Q5" s="8"/>
     </row>
     <row r="6" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A6" s="23"/>
+      <c r="A6" s="24"/>
       <c r="B6" s="4"/>
       <c r="C6" s="4"/>
       <c r="D6" s="15" t="s">
         <v>59</v>
       </c>
-      <c r="E6" s="23"/>
-      <c r="F6" s="23"/>
+      <c r="E6" s="24"/>
+      <c r="F6" s="24"/>
       <c r="G6" s="2" t="s">
         <v>115</v>
       </c>
-      <c r="H6" s="24"/>
+      <c r="H6" s="25"/>
       <c r="I6" s="2" t="s">
         <v>116</v>
       </c>
-      <c r="J6" s="25"/>
+      <c r="J6" s="26"/>
       <c r="K6" s="8"/>
       <c r="L6" s="8"/>
       <c r="M6" s="8"/>
@@ -3722,18 +3735,18 @@
       <c r="Q6" s="8"/>
     </row>
     <row r="7" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A7" s="23"/>
+      <c r="A7" s="24"/>
       <c r="B7" s="4"/>
       <c r="C7" s="4"/>
       <c r="D7" s="15" t="s">
         <v>61</v>
       </c>
-      <c r="E7" s="23"/>
-      <c r="F7" s="23"/>
-      <c r="G7" s="25"/>
-      <c r="H7" s="25"/>
-      <c r="I7" s="25"/>
-      <c r="J7" s="25"/>
+      <c r="E7" s="24"/>
+      <c r="F7" s="24"/>
+      <c r="G7" s="26"/>
+      <c r="H7" s="26"/>
+      <c r="I7" s="26"/>
+      <c r="J7" s="26"/>
       <c r="K7" s="8"/>
       <c r="L7" s="8"/>
       <c r="M7" s="8"/>
@@ -3743,7 +3756,7 @@
       <c r="Q7" s="8"/>
     </row>
     <row r="8" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A8" s="23"/>
+      <c r="A8" s="24"/>
       <c r="B8" s="4"/>
       <c r="C8" s="4"/>
       <c r="D8" s="2" t="s">
@@ -3751,10 +3764,10 @@
       </c>
       <c r="E8" s="4"/>
       <c r="F8" s="4"/>
-      <c r="G8" s="25"/>
-      <c r="H8" s="25"/>
-      <c r="I8" s="25"/>
-      <c r="J8" s="25"/>
+      <c r="G8" s="26"/>
+      <c r="H8" s="26"/>
+      <c r="I8" s="26"/>
+      <c r="J8" s="26"/>
       <c r="K8" s="8"/>
       <c r="L8" s="8"/>
       <c r="M8" s="8"/>
@@ -3767,13 +3780,13 @@
       <c r="A9" s="4"/>
       <c r="B9" s="4"/>
       <c r="C9" s="4"/>
-      <c r="D9" s="26"/>
+      <c r="D9" s="27"/>
       <c r="E9" s="4"/>
       <c r="F9" s="4"/>
-      <c r="G9" s="25"/>
-      <c r="H9" s="25"/>
-      <c r="I9" s="25"/>
-      <c r="J9" s="25"/>
+      <c r="G9" s="26"/>
+      <c r="H9" s="26"/>
+      <c r="I9" s="26"/>
+      <c r="J9" s="26"/>
       <c r="K9" s="8"/>
       <c r="L9" s="8"/>
       <c r="M9" s="8"/>
@@ -3786,13 +3799,13 @@
       <c r="A10" s="4"/>
       <c r="B10" s="4"/>
       <c r="C10" s="4"/>
-      <c r="D10" s="26"/>
+      <c r="D10" s="27"/>
       <c r="E10" s="4"/>
       <c r="F10" s="4"/>
-      <c r="G10" s="25"/>
-      <c r="H10" s="25"/>
-      <c r="I10" s="25"/>
-      <c r="J10" s="25"/>
+      <c r="G10" s="26"/>
+      <c r="H10" s="26"/>
+      <c r="I10" s="26"/>
+      <c r="J10" s="26"/>
       <c r="K10" s="8"/>
       <c r="L10" s="8"/>
       <c r="M10" s="8"/>
@@ -3805,13 +3818,13 @@
       <c r="A11" s="4"/>
       <c r="B11" s="4"/>
       <c r="C11" s="4"/>
-      <c r="D11" s="26"/>
+      <c r="D11" s="27"/>
       <c r="E11" s="4"/>
       <c r="F11" s="4"/>
-      <c r="G11" s="25"/>
-      <c r="H11" s="25"/>
-      <c r="I11" s="25"/>
-      <c r="J11" s="25"/>
+      <c r="G11" s="26"/>
+      <c r="H11" s="26"/>
+      <c r="I11" s="26"/>
+      <c r="J11" s="26"/>
       <c r="K11" s="8"/>
       <c r="L11" s="8"/>
       <c r="M11" s="8"/>
@@ -3824,13 +3837,13 @@
       <c r="A12" s="4"/>
       <c r="B12" s="4"/>
       <c r="C12" s="4"/>
-      <c r="D12" s="27"/>
+      <c r="D12" s="28"/>
       <c r="E12" s="4"/>
       <c r="F12" s="4"/>
-      <c r="G12" s="25"/>
-      <c r="H12" s="25"/>
-      <c r="I12" s="25"/>
-      <c r="J12" s="25"/>
+      <c r="G12" s="26"/>
+      <c r="H12" s="26"/>
+      <c r="I12" s="26"/>
+      <c r="J12" s="26"/>
       <c r="K12" s="8"/>
       <c r="L12" s="8"/>
       <c r="M12" s="8"/>
@@ -3843,13 +3856,13 @@
       <c r="A13" s="4"/>
       <c r="B13" s="4"/>
       <c r="C13" s="4"/>
-      <c r="D13" s="27"/>
+      <c r="D13" s="28"/>
       <c r="E13" s="4"/>
       <c r="F13" s="4"/>
-      <c r="G13" s="25"/>
-      <c r="H13" s="25"/>
-      <c r="I13" s="25"/>
-      <c r="J13" s="25"/>
+      <c r="G13" s="26"/>
+      <c r="H13" s="26"/>
+      <c r="I13" s="26"/>
+      <c r="J13" s="26"/>
       <c r="K13" s="8"/>
       <c r="L13" s="8"/>
       <c r="M13" s="8"/>

</xml_diff>